<commit_message>
Added tcmalloc spinlock data to spreadsheet
</commit_message>
<xml_diff>
--- a/paper/data4.xlsx
+++ b/paper/data4.xlsx
@@ -9,21 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="140" yWindow="520" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="3" r:id="rId1"/>
     <sheet name="mmprof" sheetId="4" r:id="rId2"/>
-    <sheet name="aget" sheetId="9" r:id="rId3"/>
-    <sheet name="blackscholes" sheetId="12" r:id="rId4"/>
-    <sheet name="bodytrack" sheetId="13" r:id="rId5"/>
-    <sheet name="Sheet8" sheetId="21" r:id="rId6"/>
+    <sheet name="tcmalloc spinlocks" sheetId="23" r:id="rId3"/>
+    <sheet name="Explaination" sheetId="22" r:id="rId4"/>
+    <sheet name="aget" sheetId="9" r:id="rId5"/>
+    <sheet name="blackscholes" sheetId="12" r:id="rId6"/>
+    <sheet name="bodytrack" sheetId="13" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="21" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="data" localSheetId="0">Baseline!$A$1:$M$17</definedName>
+    <definedName name="data" localSheetId="3">Explaination!$A$1:$M$17</definedName>
     <definedName name="data" localSheetId="1">mmprof!$A$1:$L$17</definedName>
-    <definedName name="data" localSheetId="5">Sheet8!$A$1:$R$17</definedName>
+    <definedName name="data" localSheetId="7">Sheet8!$A$1:$R$17</definedName>
     <definedName name="data_1" localSheetId="0">Baseline!$A$23:$M$39</definedName>
+    <definedName name="data_1" localSheetId="3">Explaination!$A$23:$M$39</definedName>
     <definedName name="data_1" localSheetId="1">mmprof!$A$23:$M$39</definedName>
     <definedName name="data_2" localSheetId="1">mmprof!$A$23:$L$39</definedName>
   </definedNames>
@@ -199,9 +203,10 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="data.txt3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="data.txt21" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="7">
+      <textFields count="8">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -212,30 +217,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="data.txt4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="data.txt22" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="29">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+      <textFields count="8">
         <textField/>
         <textField/>
         <textField/>
@@ -247,17 +231,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="data.txt5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="15">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="12" name="data.txt3" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
+      <textFields count="7">
         <textField/>
         <textField/>
         <textField/>
@@ -268,9 +244,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="data.txt6" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="13">
+  <connection id="13" name="data.txt4" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -287,25 +279,65 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="data.txt7" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="14" name="data.txt5" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="3">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="data.txt8" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="15" name="data.txt6" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="3">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="data.txt9" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="16" name="data.txt7" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="17" name="data.txt8" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="18" name="data.txt9" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
       <textFields count="15">
         <textField/>
@@ -330,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="82">
   <si>
     <t>benchmark</t>
   </si>
@@ -562,6 +594,21 @@
   <si>
     <t>Testname</t>
   </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>num locks</t>
+  </si>
+  <si>
+    <t>num waits</t>
+  </si>
+  <si>
+    <t>time wait</t>
+  </si>
+  <si>
+    <t>max cont</t>
+  </si>
 </sst>
 </file>
 
@@ -668,8 +715,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="649">
+  <cellStyleXfs count="653">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1338,7 +1389,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="649">
+  <cellStyles count="653">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1663,6 +1714,8 @@
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1987,6 +2040,8 @@
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2008,11 +2063,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_2" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_2" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2020,6 +2075,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2347,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4391,8 +4454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5355,6 +5418,12 @@
         <v>2.8800650872009901</v>
       </c>
     </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <f>AVERAGE(C18,E18,G18,I18,K18,M18,O18)</f>
+        <v>3.129732444186812</v>
+      </c>
+    </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>27</v>
@@ -6331,6 +6400,2341 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>2271488</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <v>46718</v>
+      </c>
+      <c r="D3">
+        <v>15372071</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>1127842</v>
+      </c>
+      <c r="D4">
+        <v>119483700</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>89</v>
+      </c>
+      <c r="C5">
+        <v>247963</v>
+      </c>
+      <c r="D5">
+        <v>46644064</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>89</v>
+      </c>
+      <c r="C6">
+        <v>99845</v>
+      </c>
+      <c r="D6">
+        <v>10840976</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>89</v>
+      </c>
+      <c r="C7">
+        <v>16636</v>
+      </c>
+      <c r="D7">
+        <v>6332771</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>36880</v>
+      </c>
+      <c r="D8">
+        <v>4520763</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>13007</v>
+      </c>
+      <c r="D9">
+        <v>15279663</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1979</v>
+      </c>
+      <c r="D10">
+        <v>15081407</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>170406</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>451047</v>
+      </c>
+      <c r="D12">
+        <v>39771993</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>454</v>
+      </c>
+      <c r="D13">
+        <v>988233</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>1253</v>
+      </c>
+      <c r="D14">
+        <v>1741829</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>59</v>
+      </c>
+      <c r="C15">
+        <v>908</v>
+      </c>
+      <c r="D15">
+        <v>159594</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>5258</v>
+      </c>
+      <c r="D16">
+        <v>1163362</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D11">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.49</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D9" si="0">C2/$B2</f>
+        <v>1.0018214936247722</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="F2" s="2">
+        <f>E2/$B2</f>
+        <v>1.0018214936247722</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5.49</v>
+      </c>
+      <c r="H2" s="1">
+        <f>G2/$B2</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5.49</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" ref="J2:J17" si="1">I2/$B2</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>5.49</v>
+      </c>
+      <c r="L2" s="1">
+        <f>K2/$B2</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" ref="N2:N17" si="2">M2/$B2</f>
+        <v>1.0018214936247722</v>
+      </c>
+      <c r="O2" s="1">
+        <v>5.49</v>
+      </c>
+      <c r="P2" s="1">
+        <f>O2/$B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>60.52</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60.52</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>61.19</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F17" si="3">E3/$B3</f>
+        <v>1.0110707204230005</v>
+      </c>
+      <c r="G3" s="1">
+        <v>60.85</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H4" si="4">G3/$B3</f>
+        <v>1.0054527428949107</v>
+      </c>
+      <c r="I3" s="2">
+        <v>61.2</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0112359550561798</v>
+      </c>
+      <c r="K3" s="1">
+        <v>60.58</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L4" si="5">K3/$B3</f>
+        <v>1.0009914077990747</v>
+      </c>
+      <c r="M3" s="2">
+        <v>60.89</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0061136814276272</v>
+      </c>
+      <c r="O3" s="1">
+        <v>61.35</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P4" si="6">O3/$B3</f>
+        <v>1.0137144745538664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>31.62</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31.54</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.99746995572422514</v>
+      </c>
+      <c r="E4" s="2">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="3"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="G4" s="1">
+        <v>31.9</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0088551549652118</v>
+      </c>
+      <c r="I4" s="2">
+        <v>31.46</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9949399114484504</v>
+      </c>
+      <c r="K4" s="1">
+        <v>31.69</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="5"/>
+        <v>1.002213788741303</v>
+      </c>
+      <c r="M4" s="2">
+        <v>31.67</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0015812776723594</v>
+      </c>
+      <c r="O4" s="1">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="6"/>
+        <v>1.0553447185325742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>61.35</v>
+      </c>
+      <c r="C5" s="1">
+        <v>57.03</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.92958435207823964</v>
+      </c>
+      <c r="E5" s="2">
+        <v>92.84</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="3"/>
+        <v>1.5132844335778322</v>
+      </c>
+      <c r="G5" s="1">
+        <v>57.54</v>
+      </c>
+      <c r="H5" s="9">
+        <f>G5/$B5</f>
+        <v>0.93789731051344738</v>
+      </c>
+      <c r="I5" s="2">
+        <v>60.39</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9843520782396088</v>
+      </c>
+      <c r="K5" s="1">
+        <v>61.52</v>
+      </c>
+      <c r="L5" s="10">
+        <f>K5/$B5</f>
+        <v>1.0027709861450693</v>
+      </c>
+      <c r="M5" s="2">
+        <v>61.48</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0021189894050528</v>
+      </c>
+      <c r="O5" s="1">
+        <v>67.150000000000006</v>
+      </c>
+      <c r="P5" s="9">
+        <f>O5/$B5</f>
+        <v>1.0945395273023635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12.51</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10.23</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.81774580335731417</v>
+      </c>
+      <c r="E6" s="2">
+        <v>27.64</v>
+      </c>
+      <c r="F6" s="9">
+        <f>E6/$B6</f>
+        <v>2.2094324540367705</v>
+      </c>
+      <c r="G6" s="1">
+        <v>10.58</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" ref="H6:L17" si="7">G6/$B6</f>
+        <v>0.84572342126298961</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10.39</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="7"/>
+        <v>0.8305355715427658</v>
+      </c>
+      <c r="K6" s="1">
+        <v>16.53</v>
+      </c>
+      <c r="L6" s="9">
+        <f>K6/$B6</f>
+        <v>1.3213429256594726</v>
+      </c>
+      <c r="M6" s="2">
+        <v>12.67</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0127897681854516</v>
+      </c>
+      <c r="O6" s="1">
+        <v>23.35</v>
+      </c>
+      <c r="P6" s="9">
+        <f>O6/$B6</f>
+        <v>1.8665067945643488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>89.06</v>
+      </c>
+      <c r="C7" s="1">
+        <v>90.21</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0129126431619133</v>
+      </c>
+      <c r="E7" s="2">
+        <v>101.41</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1386705591735908</v>
+      </c>
+      <c r="G7" s="1">
+        <v>91.12</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0231304738378622</v>
+      </c>
+      <c r="I7" s="2">
+        <v>87.73</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.98506624747361327</v>
+      </c>
+      <c r="K7" s="1">
+        <v>88.59</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" ref="L7:L17" si="8">K7/$B7</f>
+        <v>0.99472265888165279</v>
+      </c>
+      <c r="M7" s="2">
+        <v>89.2</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0015719739501461</v>
+      </c>
+      <c r="O7" s="1">
+        <v>91.05</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" ref="P7:P17" si="9">O7/$B7</f>
+        <v>1.0223444868627891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4.68</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.72</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0085470085470085</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.83</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0320512820512822</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.71</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0064102564102564</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0042735042735045</v>
+      </c>
+      <c r="K8" s="1">
+        <v>4.68</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0042735042735045</v>
+      </c>
+      <c r="O8" s="1">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="9"/>
+        <v>1.0106837606837609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
+        <v>37.96</v>
+      </c>
+      <c r="C9" s="1">
+        <v>39.409999999999997</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0381981032665963</v>
+      </c>
+      <c r="E9" s="2">
+        <v>38.47</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0134351949420441</v>
+      </c>
+      <c r="G9" s="1">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="7"/>
+        <v>0.95258166491043195</v>
+      </c>
+      <c r="I9" s="2">
+        <v>38.29</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0086933614330875</v>
+      </c>
+      <c r="K9" s="1">
+        <v>38.65</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="8"/>
+        <v>1.018177028451001</v>
+      </c>
+      <c r="M9" s="2">
+        <v>39.86</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0500526870389884</v>
+      </c>
+      <c r="O9" s="1">
+        <v>37.08</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="9"/>
+        <v>0.97681770284510006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>54.45</v>
+      </c>
+      <c r="C10" s="1">
+        <v>25.35</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="2">
+        <v>185.08</v>
+      </c>
+      <c r="F10" s="9">
+        <f>E10/$B10</f>
+        <v>3.3990817263544537</v>
+      </c>
+      <c r="G10" s="1">
+        <v>56.3</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0339761248852157</v>
+      </c>
+      <c r="I10" s="2">
+        <v>54.77</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0058769513314967</v>
+      </c>
+      <c r="K10" s="1">
+        <v>53.79</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="8"/>
+        <v>0.9878787878787878</v>
+      </c>
+      <c r="M10" s="2">
+        <v>54.73</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0051423324150597</v>
+      </c>
+      <c r="O10" s="1">
+        <v>52.08</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="9"/>
+        <v>0.9564738292011018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.62</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" ref="D11:D17" si="10">C11/$B11</f>
+        <v>0.96913580246913578</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.65</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0185185185185184</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="7"/>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.58</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="8"/>
+        <v>0.97530864197530864</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.61</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99382716049382713</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="9"/>
+        <v>0.96913580246913578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>53.58</v>
+      </c>
+      <c r="C12" s="1">
+        <v>53.63</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0009331840238895</v>
+      </c>
+      <c r="E12" s="2">
+        <v>54.09</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0095184770436731</v>
+      </c>
+      <c r="G12" s="1">
+        <v>54.33</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0139977603583428</v>
+      </c>
+      <c r="I12" s="2">
+        <v>54.71</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.021089958939903</v>
+      </c>
+      <c r="K12" s="1">
+        <v>54.73</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="8"/>
+        <v>1.0214632325494588</v>
+      </c>
+      <c r="M12" s="2">
+        <v>54.54</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0179171332586787</v>
+      </c>
+      <c r="O12" s="1">
+        <v>53.82</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="9"/>
+        <v>1.0044792833146696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3">
+        <v>90.65</v>
+      </c>
+      <c r="C13" s="1">
+        <v>82.53</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="10"/>
+        <v>0.9104247104247104</v>
+      </c>
+      <c r="E13" s="2">
+        <v>102.55</v>
+      </c>
+      <c r="F13" s="2">
+        <f>E13/$B13</f>
+        <v>1.1312741312741312</v>
+      </c>
+      <c r="G13" s="1">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="7"/>
+        <v>0.77109762824048544</v>
+      </c>
+      <c r="I13" s="2">
+        <v>86.02</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="7"/>
+        <v>0.94892443463872023</v>
+      </c>
+      <c r="K13" s="1">
+        <v>93.89</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="7"/>
+        <v>1.0357418643132927</v>
+      </c>
+      <c r="M13" s="2">
+        <v>93.62</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0327633756205186</v>
+      </c>
+      <c r="O13" s="1">
+        <v>80.52</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.88825151682294534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>54.02</v>
+      </c>
+      <c r="C14" s="1">
+        <v>55.44</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0262865605331357</v>
+      </c>
+      <c r="E14" s="2">
+        <v>54.01</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.99981488337652713</v>
+      </c>
+      <c r="G14" s="1">
+        <v>53.93</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="7"/>
+        <v>0.99833395038874484</v>
+      </c>
+      <c r="I14" s="2">
+        <v>55.45</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0264716771566087</v>
+      </c>
+      <c r="K14" s="1">
+        <v>53.57</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="8"/>
+        <v>0.99166975194372453</v>
+      </c>
+      <c r="M14" s="2">
+        <v>53.67</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99352091817845245</v>
+      </c>
+      <c r="O14" s="1">
+        <v>54.17</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="9"/>
+        <v>1.0027767493520918</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3">
+        <v>36.89</v>
+      </c>
+      <c r="C15" s="1">
+        <v>40.9</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1087015451341826</v>
+      </c>
+      <c r="E15" s="2">
+        <v>163.43</v>
+      </c>
+      <c r="F15" s="9">
+        <f>E15/$B15</f>
+        <v>4.430197885605855</v>
+      </c>
+      <c r="G15" s="1">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0336134453781514</v>
+      </c>
+      <c r="I15" s="2">
+        <v>36.81</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99783139062076454</v>
+      </c>
+      <c r="K15" s="1">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="8"/>
+        <v>1.0151802656546489</v>
+      </c>
+      <c r="M15" s="2">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0159934941718622</v>
+      </c>
+      <c r="O15" s="1">
+        <v>99.22</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" si="9"/>
+        <v>2.6896177825969096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3">
+        <v>116.67</v>
+      </c>
+      <c r="C16" s="1">
+        <v>115.89</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="10"/>
+        <v>0.99331447672923634</v>
+      </c>
+      <c r="E16" s="2">
+        <v>121.99</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0455986971800806</v>
+      </c>
+      <c r="G16" s="1">
+        <v>115.71</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="7"/>
+        <v>0.99177166366675229</v>
+      </c>
+      <c r="I16" s="2">
+        <v>116.35</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99725722122225069</v>
+      </c>
+      <c r="K16" s="1">
+        <v>116.79</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="8"/>
+        <v>1.001028542041656</v>
+      </c>
+      <c r="M16" s="2">
+        <v>116.78</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0009428302048513</v>
+      </c>
+      <c r="O16" s="1">
+        <v>119.32</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="9"/>
+        <v>1.0227136367532355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
+        <v>50.66</v>
+      </c>
+      <c r="C17" s="1">
+        <v>50.77</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="10"/>
+        <v>1.0021713383339914</v>
+      </c>
+      <c r="E17" s="2">
+        <v>50.92</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0051322542439796</v>
+      </c>
+      <c r="G17" s="1">
+        <v>50.46</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="7"/>
+        <v>0.99605211212001588</v>
+      </c>
+      <c r="I17" s="2">
+        <v>50.28</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99249901302803012</v>
+      </c>
+      <c r="K17" s="1">
+        <v>50.66</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
+        <v>50.64</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99960521121200163</v>
+      </c>
+      <c r="O17" s="1">
+        <v>50.45</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="9"/>
+        <v>0.99585471772601675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1">
+        <f>AVERAGE(D2:D17)</f>
+        <v>0.98781646516055654</v>
+      </c>
+      <c r="F18" s="2">
+        <f>AVERAGE(F2:F17)</f>
+        <v>1.5021357205394259</v>
+      </c>
+      <c r="H18" s="1">
+        <f>AVERAGE(H2:H17)</f>
+        <v>0.97270863464232882</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
+        <f>AVERAGE(J2:J17)</f>
+        <v>0.98806545477531138</v>
+      </c>
+      <c r="L18" s="1">
+        <f>AVERAGE(L2:L17)</f>
+        <v>1.0230306176271533</v>
+      </c>
+      <c r="N18" s="2">
+        <f>AVERAGE(N2:N17)</f>
+        <v>1.0087522394458224</v>
+      </c>
+      <c r="P18" s="1">
+        <f>AVERAGE(P2:P17)</f>
+        <v>1.1605784239738066</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4416</v>
+      </c>
+      <c r="C24" s="1">
+        <v>68174</v>
+      </c>
+      <c r="D24" s="1">
+        <f>C24/$B24</f>
+        <v>15.437952898550725</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5822</v>
+      </c>
+      <c r="F24" s="2">
+        <f>E24/$B24</f>
+        <v>1.3183876811594204</v>
+      </c>
+      <c r="G24" s="1">
+        <v>9322</v>
+      </c>
+      <c r="H24" s="1">
+        <f>G24/$B24</f>
+        <v>2.1109601449275361</v>
+      </c>
+      <c r="I24" s="2">
+        <v>33195</v>
+      </c>
+      <c r="J24" s="2">
+        <f>I24/$B24</f>
+        <v>7.5169836956521738</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4711</v>
+      </c>
+      <c r="L24" s="1">
+        <f>K24/$B24</f>
+        <v>1.066802536231884</v>
+      </c>
+      <c r="M24" s="2">
+        <v>4982</v>
+      </c>
+      <c r="N24" s="2">
+        <f>M24/$B24</f>
+        <v>1.1281702898550725</v>
+      </c>
+      <c r="O24" s="1">
+        <v>3407</v>
+      </c>
+      <c r="P24" s="1">
+        <f>O24/$B24</f>
+        <v>0.77151268115942029</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>628103</v>
+      </c>
+      <c r="C25" s="1">
+        <v>647403</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D39" si="11">C25/$B25</f>
+        <v>1.0307274443841217</v>
+      </c>
+      <c r="E25" s="2">
+        <v>634200</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F39" si="12">E25/$B25</f>
+        <v>1.0097070066533673</v>
+      </c>
+      <c r="G25" s="1">
+        <v>635214</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H39" si="13">G25/$B25</f>
+        <v>1.0113213915552066</v>
+      </c>
+      <c r="I25" s="2">
+        <v>640453</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" ref="J25:J39" si="14">I25/$B25</f>
+        <v>1.01966238021471</v>
+      </c>
+      <c r="K25" s="1">
+        <v>627813</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" ref="L25:L39" si="15">K25/$B25</f>
+        <v>0.99953829228645619</v>
+      </c>
+      <c r="M25" s="2">
+        <v>627347</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" ref="N25:N39" si="16">M25/$B25</f>
+        <v>0.99879637575365821</v>
+      </c>
+      <c r="O25" s="1">
+        <v>628312</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" ref="P25:P39" si="17">O25/$B25</f>
+        <v>1.0003327479728643</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3">
+        <v>34266</v>
+      </c>
+      <c r="C26" s="1">
+        <v>201742</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="11"/>
+        <v>5.8875269946886126</v>
+      </c>
+      <c r="E26" s="2">
+        <v>42270</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="12"/>
+        <v>1.2335843109788127</v>
+      </c>
+      <c r="G26" s="1">
+        <v>41994</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="13"/>
+        <v>1.2255296795657502</v>
+      </c>
+      <c r="I26" s="2">
+        <v>55996</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="14"/>
+        <v>1.6341563065429288</v>
+      </c>
+      <c r="K26" s="1">
+        <v>34522</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="15"/>
+        <v>1.0074709624700871</v>
+      </c>
+      <c r="M26" s="2">
+        <v>34526</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0075876962586821</v>
+      </c>
+      <c r="O26" s="1">
+        <v>32318</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" si="17"/>
+        <v>0.94315064495418199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3">
+        <v>966256</v>
+      </c>
+      <c r="C27" s="1">
+        <v>857162</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="11"/>
+        <v>0.88709617327085166</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1158054</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="12"/>
+        <v>1.1984960507360369</v>
+      </c>
+      <c r="G27" s="1">
+        <v>779726</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="13"/>
+        <v>0.80695592058419296</v>
+      </c>
+      <c r="I27" s="2">
+        <v>965594</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="14"/>
+        <v>0.99931488135649349</v>
+      </c>
+      <c r="K27" s="1">
+        <v>966215</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99995756818068915</v>
+      </c>
+      <c r="M27" s="2">
+        <v>966230</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="16"/>
+        <v>0.99997309201702245</v>
+      </c>
+      <c r="O27" s="1">
+        <v>828530</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="17"/>
+        <v>0.85746427447798512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1544115</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2107986</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="11"/>
+        <v>1.3651742260129589</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2107256</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="12"/>
+        <v>1.3647014632977466</v>
+      </c>
+      <c r="G28" s="1">
+        <v>905685</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="13"/>
+        <v>0.58653986263976454</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1687977</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0931679311450249</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1710884</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="15"/>
+        <v>1.1080029661003228</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1558874</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0095582259093396</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1031577</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="17"/>
+        <v>0.66807005954867349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2501287</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3543776</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="11"/>
+        <v>1.4167810411200314</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3582350</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="12"/>
+        <v>1.4322027020489851</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2585988</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="13"/>
+        <v>1.0338629673444111</v>
+      </c>
+      <c r="I29" s="2">
+        <v>2887186</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="14"/>
+        <v>1.1542801765651043</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2500269</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99959300951869978</v>
+      </c>
+      <c r="M29" s="2">
+        <v>2499812</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="16"/>
+        <v>0.99941030357571925</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2579716</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0313554582101134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3">
+        <v>68818</v>
+      </c>
+      <c r="C30" s="1">
+        <v>294836</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="11"/>
+        <v>4.2842860879421085</v>
+      </c>
+      <c r="E30" s="2">
+        <v>94872</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="12"/>
+        <v>1.3785928100206342</v>
+      </c>
+      <c r="G30" s="1">
+        <v>79288</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="13"/>
+        <v>1.1521404283762968</v>
+      </c>
+      <c r="I30" s="2">
+        <v>82326</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="14"/>
+        <v>1.1962858554447964</v>
+      </c>
+      <c r="K30" s="1">
+        <v>70226</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="15"/>
+        <v>1.0204597634339854</v>
+      </c>
+      <c r="M30" s="2">
+        <v>69086</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0038943299718097</v>
+      </c>
+      <c r="O30" s="1">
+        <v>70388</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0228137987154524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="3">
+        <v>418242</v>
+      </c>
+      <c r="C31" s="1">
+        <v>456146</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="11"/>
+        <v>1.0906269575987109</v>
+      </c>
+      <c r="E31" s="2">
+        <v>475282</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="12"/>
+        <v>1.1363803730854385</v>
+      </c>
+      <c r="G31" s="1">
+        <v>427996</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="13"/>
+        <v>1.0233214263512511</v>
+      </c>
+      <c r="I31" s="2">
+        <v>418066</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="14"/>
+        <v>0.99957919099468728</v>
+      </c>
+      <c r="K31" s="1">
+        <v>418065</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99957680003442984</v>
+      </c>
+      <c r="M31" s="2">
+        <v>418554</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0007459796003271</v>
+      </c>
+      <c r="O31" s="1">
+        <v>440655</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0535885922504196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1506831</v>
+      </c>
+      <c r="C32" s="1">
+        <v>642414</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="11"/>
+        <v>0.42633447281081954</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1167073</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="12"/>
+        <v>0.7745214957749077</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1121526</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="13"/>
+        <v>0.74429448292476064</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1511559</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0031377108647221</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1510505</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="15"/>
+        <v>1.0024382296355729</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1507155</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0002150207952982</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1100256</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="17"/>
+        <v>0.73017876590009101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="3">
+        <v>244495</v>
+      </c>
+      <c r="C33" s="1">
+        <v>295654</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="11"/>
+        <v>1.2092435428127364</v>
+      </c>
+      <c r="E33" s="2">
+        <v>252745</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0337430213296794</v>
+      </c>
+      <c r="G33" s="1">
+        <v>274665</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="13"/>
+        <v>1.1233972064868403</v>
+      </c>
+      <c r="I33" s="2">
+        <v>244572</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0003149348657436</v>
+      </c>
+      <c r="K33" s="1">
+        <v>244432</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99974232601893698</v>
+      </c>
+      <c r="M33" s="2">
+        <v>245152</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0026871715168</v>
+      </c>
+      <c r="O33" s="1">
+        <v>255081</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0432974089449683</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
+        <v>845040</v>
+      </c>
+      <c r="C34" s="1">
+        <v>866451</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="11"/>
+        <v>1.0253372621414372</v>
+      </c>
+      <c r="E34" s="2">
+        <v>849418</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0051808198428476</v>
+      </c>
+      <c r="G34" s="1">
+        <v>852298</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="13"/>
+        <v>1.0085889425352645</v>
+      </c>
+      <c r="I34" s="2">
+        <v>857540</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0147921991858373</v>
+      </c>
+      <c r="K34" s="1">
+        <v>844810</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99972782353498058</v>
+      </c>
+      <c r="M34" s="2">
+        <v>845453</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0004887342611</v>
+      </c>
+      <c r="O34" s="1">
+        <v>847792</v>
+      </c>
+      <c r="P34" s="1">
+        <f t="shared" si="17"/>
+        <v>1.003256650572754</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1162004</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1568268</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="11"/>
+        <v>1.3496235813301847</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1722894</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="12"/>
+        <v>1.4826919700792769</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1115487</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="13"/>
+        <v>0.95996829615044355</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1665620</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="14"/>
+        <v>1.4334029831222612</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1161856</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99987263382914349</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1162131</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0001092939439107</v>
+      </c>
+      <c r="O35" s="1">
+        <v>1110797</v>
+      </c>
+      <c r="P35" s="1">
+        <f t="shared" si="17"/>
+        <v>0.95593216546586757</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="3">
+        <v>114473</v>
+      </c>
+      <c r="C36" s="1">
+        <v>139023</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="11"/>
+        <v>1.2144610519511152</v>
+      </c>
+      <c r="E36" s="2">
+        <v>117356</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0251849781171105</v>
+      </c>
+      <c r="G36" s="1">
+        <v>122510</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="13"/>
+        <v>1.070208695500249</v>
+      </c>
+      <c r="I36" s="2">
+        <v>122963</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0741659605321778</v>
+      </c>
+      <c r="K36" s="1">
+        <v>113747</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99365789312763708</v>
+      </c>
+      <c r="M36" s="2">
+        <v>116693</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="16"/>
+        <v>1.019393219361771</v>
+      </c>
+      <c r="O36" s="1">
+        <v>114693</v>
+      </c>
+      <c r="P36" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0019218505673828</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="3">
+        <v>9860</v>
+      </c>
+      <c r="C37" s="1">
+        <v>165203</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="11"/>
+        <v>16.754868154158213</v>
+      </c>
+      <c r="E37" s="2">
+        <v>11508</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="12"/>
+        <v>1.1671399594320486</v>
+      </c>
+      <c r="G37" s="1">
+        <v>13770</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="13"/>
+        <v>1.396551724137931</v>
+      </c>
+      <c r="I37" s="2">
+        <v>42382</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="14"/>
+        <v>4.2983772819472614</v>
+      </c>
+      <c r="K37" s="1">
+        <v>10120</v>
+      </c>
+      <c r="L37" s="1">
+        <f t="shared" si="15"/>
+        <v>1.026369168356998</v>
+      </c>
+      <c r="M37" s="2">
+        <v>9300</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="16"/>
+        <v>0.94320486815415816</v>
+      </c>
+      <c r="O37" s="1">
+        <v>7621</v>
+      </c>
+      <c r="P37" s="1">
+        <f t="shared" si="17"/>
+        <v>0.77292089249492901</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="3">
+        <v>31504</v>
+      </c>
+      <c r="C38" s="1">
+        <v>59560</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="11"/>
+        <v>1.8905535804977145</v>
+      </c>
+      <c r="E38" s="2">
+        <v>36086</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="12"/>
+        <v>1.1454418486541391</v>
+      </c>
+      <c r="G38" s="1">
+        <v>39450</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="13"/>
+        <v>1.2522219400711021</v>
+      </c>
+      <c r="I38" s="2">
+        <v>40158</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="14"/>
+        <v>1.2746952767902489</v>
+      </c>
+      <c r="K38" s="1">
+        <v>31791</v>
+      </c>
+      <c r="L38" s="1">
+        <f t="shared" si="15"/>
+        <v>1.0091099542915185</v>
+      </c>
+      <c r="M38" s="2">
+        <v>31815</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0098717623158964</v>
+      </c>
+      <c r="O38" s="1">
+        <v>32044</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0171406805485017</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3">
+        <v>496521</v>
+      </c>
+      <c r="C39" s="1">
+        <v>552222</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="11"/>
+        <v>1.1121825662962896</v>
+      </c>
+      <c r="E39" s="2">
+        <v>529431</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0662811844816231</v>
+      </c>
+      <c r="G39" s="1">
+        <v>515456</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="13"/>
+        <v>1.0381353457356286</v>
+      </c>
+      <c r="I39" s="2">
+        <v>609121</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="14"/>
+        <v>1.2267779207727367</v>
+      </c>
+      <c r="K39" s="1">
+        <v>498261</v>
+      </c>
+      <c r="L39" s="1">
+        <f t="shared" si="15"/>
+        <v>1.0035043835003958</v>
+      </c>
+      <c r="M39" s="2">
+        <v>498224</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="16"/>
+        <v>1.0034298650006748</v>
+      </c>
+      <c r="O39" s="1">
+        <v>517812</v>
+      </c>
+      <c r="P39" s="1">
+        <f t="shared" si="17"/>
+        <v>1.0428803615557045</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1">
+        <f>SUM(C24:C39)/SUM($B24:$B39)</f>
+        <v>1.1786826516932165</v>
+      </c>
+      <c r="F40" s="2">
+        <f>SUM(E24:E39)/SUM($B24:$B39)</f>
+        <v>1.2089956242445914</v>
+      </c>
+      <c r="H40" s="1">
+        <f>SUM(G24:G39)/SUM($B24:$B39)</f>
+        <v>0.90016708220537167</v>
+      </c>
+      <c r="J40" s="2">
+        <f>SUM(I24:I39)/SUM($B24:$B39)</f>
+        <v>1.1218276151494799</v>
+      </c>
+      <c r="L40" s="1">
+        <f>SUM(K24:K39)/SUM($B24:$B39)</f>
+        <v>1.0162625040999955</v>
+      </c>
+      <c r="N40" s="2">
+        <f>SUM(M24:M39)/SUM($B24:$B39)</f>
+        <v>1.0018062200040827</v>
+      </c>
+      <c r="P40" s="1">
+        <f>SUM(O24:O39)/SUM($B24:$B39)</f>
+        <v>0.90779021373493074</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A22:P22"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
@@ -7425,7 +9829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
@@ -8830,7 +11234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
@@ -9163,7 +11567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added new (but bad) data to spreadsheet
</commit_message>
<xml_diff>
--- a/paper/data4.xlsx
+++ b/paper/data4.xlsx
@@ -5,31 +5,33 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/mmprof/paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/MallocProfiler/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="140" yWindow="520" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="3" r:id="rId1"/>
-    <sheet name="mmprof" sheetId="4" r:id="rId2"/>
-    <sheet name="tcmalloc spinlocks" sheetId="23" r:id="rId3"/>
-    <sheet name="Explaination" sheetId="22" r:id="rId4"/>
-    <sheet name="aget" sheetId="9" r:id="rId5"/>
-    <sheet name="blackscholes" sheetId="12" r:id="rId6"/>
-    <sheet name="bodytrack" sheetId="13" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="21" r:id="rId8"/>
+    <sheet name="mmprof new experimental" sheetId="24" r:id="rId2"/>
+    <sheet name="mmprof" sheetId="4" r:id="rId3"/>
+    <sheet name="tcmalloc spinlocks" sheetId="23" r:id="rId4"/>
+    <sheet name="Explaination" sheetId="22" r:id="rId5"/>
+    <sheet name="aget" sheetId="9" r:id="rId6"/>
+    <sheet name="blackscholes" sheetId="12" r:id="rId7"/>
+    <sheet name="bodytrack" sheetId="13" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="21" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="data" localSheetId="0">Baseline!$A$1:$M$17</definedName>
-    <definedName name="data" localSheetId="3">Explaination!$A$1:$M$17</definedName>
-    <definedName name="data" localSheetId="1">mmprof!$A$1:$L$17</definedName>
-    <definedName name="data" localSheetId="7">Sheet8!$A$1:$R$17</definedName>
+    <definedName name="data" localSheetId="4">Explaination!$A$1:$M$17</definedName>
+    <definedName name="data" localSheetId="2">mmprof!$A$1:$L$17</definedName>
+    <definedName name="data" localSheetId="1">'mmprof new experimental'!$A$2:$Y$18</definedName>
+    <definedName name="data" localSheetId="8">Sheet8!$A$1:$R$17</definedName>
     <definedName name="data_1" localSheetId="0">Baseline!$A$23:$M$39</definedName>
-    <definedName name="data_1" localSheetId="3">Explaination!$A$23:$M$39</definedName>
-    <definedName name="data_1" localSheetId="1">mmprof!$A$23:$M$39</definedName>
-    <definedName name="data_2" localSheetId="1">mmprof!$A$23:$L$39</definedName>
+    <definedName name="data_1" localSheetId="4">Explaination!$A$23:$M$39</definedName>
+    <definedName name="data_1" localSheetId="2">mmprof!$A$23:$M$39</definedName>
+    <definedName name="data_2" localSheetId="2">mmprof!$A$23:$L$39</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -45,9 +47,19 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="data.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="8">
+  <connection id="1" name="data" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sam/data.txt" delimiter="|">
+      <textFields count="18">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -59,9 +71,10 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="data.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="data.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="7">
+      <textFields count="8">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -72,17 +85,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="data.txt10" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="15">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="3" name="data.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
+      <textFields count="7">
         <textField/>
         <textField/>
         <textField/>
@@ -93,7 +98,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="data.txt11" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="data.txt10" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
       <textFields count="15">
         <textField/>
@@ -114,7 +119,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="data.txt12" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="data.txt11" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
       <textFields count="15">
         <textField/>
@@ -135,41 +140,38 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="data.txt13" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="2">
+  <connection id="6" name="data.txt12" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="data.txt14" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="16">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="7" name="data.txt13" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
+      <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="data.txt15" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="data.txt14" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="18">
-        <textField/>
-        <textField/>
+      <textFields count="16">
         <textField/>
         <textField/>
         <textField/>
@@ -189,9 +191,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="data.txt2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="8">
+  <connection id="9" name="data.txt15" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -203,7 +215,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="data.txt21" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="data.txt2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
@@ -217,7 +229,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="data.txt22" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="data.txt21" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
@@ -231,9 +243,10 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="data.txt3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="12" name="data.txt22" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="7">
+      <textFields count="8">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -244,31 +257,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="data.txt4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="data.txt3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
-      <textFields count="29">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+      <textFields count="7">
         <textField/>
         <textField/>
         <textField/>
@@ -279,9 +270,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="data.txt5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="15">
+  <connection id="14" name="data.txt4" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -300,9 +305,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="data.txt6" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="15" name="data.txt5" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="13">
+      <textFields count="15">
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -319,16 +326,26 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="data.txt7" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="16" name="data.txt6" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
-      <textFields count="3">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="data.txt8" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="17" name="data.txt7" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
       <textFields count="3">
         <textField/>
@@ -337,7 +354,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" name="data.txt9" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="18" name="data.txt8" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="19" name="data.txt9" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Mac OS X:Users:sam:Documents:data.txt" space="1" consecutive="1" delimiter="|">
       <textFields count="15">
         <textField/>
@@ -362,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="111">
   <si>
     <t>benchmark</t>
   </si>
@@ -609,6 +635,93 @@
   <si>
     <t>max cont</t>
   </si>
+  <si>
+    <t xml:space="preserve">                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test name          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cmalloc224 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    pthread </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      hoard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   tcmalloc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    omalloc </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cmalloc221 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   jemalloc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  dieharder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blackscholes       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bodytrack          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">canneal            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dedup              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">facesim            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferret             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluidanimate       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">freqmine           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pbzip2             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pfscan             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">raytrace           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">streamcluster      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">swaptions          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vips               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x264               </t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>SRG1, 2019-07-19 12:15:30, 10 runs, maprof</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -715,7 +828,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="653">
+  <cellStyleXfs count="655">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1369,8 +1482,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1388,8 +1503,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="653">
+  <cellStyles count="655">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1716,6 +1838,7 @@
     <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2042,6 +2165,7 @@
     <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2055,35 +2179,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_2" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_2" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2410,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4452,10 +4580,1425 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>58.3</v>
+      </c>
+      <c r="C4">
+        <v>65.25</v>
+      </c>
+      <c r="D4">
+        <f>C4/$B4</f>
+        <v>1.1192109777015438</v>
+      </c>
+      <c r="E4">
+        <v>65.16</v>
+      </c>
+      <c r="F4">
+        <f>E4/$B4</f>
+        <v>1.1176672384219555</v>
+      </c>
+      <c r="G4">
+        <v>65.05</v>
+      </c>
+      <c r="H4">
+        <f>G4/$B4</f>
+        <v>1.1157804459691252</v>
+      </c>
+      <c r="I4">
+        <v>65.25</v>
+      </c>
+      <c r="J4">
+        <f>I4/$B4</f>
+        <v>1.1192109777015438</v>
+      </c>
+      <c r="K4">
+        <v>65.22</v>
+      </c>
+      <c r="L4">
+        <f>K4/$B4</f>
+        <v>1.1186963979416811</v>
+      </c>
+      <c r="M4">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="N4">
+        <f>M4/$B4</f>
+        <v>1.1217838765008579</v>
+      </c>
+      <c r="O4">
+        <v>65.98</v>
+      </c>
+      <c r="P4">
+        <f>O4/$B4</f>
+        <v>1.1317324185248714</v>
+      </c>
+      <c r="Q4">
+        <v>627176</v>
+      </c>
+      <c r="R4">
+        <v>754552</v>
+      </c>
+      <c r="S4">
+        <v>801496</v>
+      </c>
+      <c r="T4">
+        <v>751640</v>
+      </c>
+      <c r="U4">
+        <v>744096</v>
+      </c>
+      <c r="V4">
+        <v>756728</v>
+      </c>
+      <c r="W4">
+        <v>784656</v>
+      </c>
+      <c r="X4">
+        <v>753300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C5">
+        <v>59.57</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D18" si="0">C5/$B5</f>
+        <v>1.6875354107648726</v>
+      </c>
+      <c r="E5">
+        <v>59.34</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F18" si="1">E5/$B5</f>
+        <v>1.6810198300283288</v>
+      </c>
+      <c r="G5">
+        <v>59.17</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H18" si="2">G5/$B5</f>
+        <v>1.676203966005666</v>
+      </c>
+      <c r="I5">
+        <v>63.08</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J18" si="3">I5/$B5</f>
+        <v>1.7869688385269122</v>
+      </c>
+      <c r="K5">
+        <v>60.88</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L18" si="4">K5/$B5</f>
+        <v>1.7246458923512751</v>
+      </c>
+      <c r="M5">
+        <v>59.31</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N18" si="5">M5/$B5</f>
+        <v>1.6801699716713883</v>
+      </c>
+      <c r="O5">
+        <v>65.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P18" si="6">O5/$B5</f>
+        <v>1.8640226628895185</v>
+      </c>
+      <c r="Q5">
+        <v>34188</v>
+      </c>
+      <c r="R5">
+        <v>87576</v>
+      </c>
+      <c r="S5">
+        <v>247392</v>
+      </c>
+      <c r="T5">
+        <v>90116</v>
+      </c>
+      <c r="U5">
+        <v>82760</v>
+      </c>
+      <c r="V5">
+        <v>92156</v>
+      </c>
+      <c r="W5">
+        <v>104420</v>
+      </c>
+      <c r="X5">
+        <v>90496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6">
+        <v>53.43</v>
+      </c>
+      <c r="C6">
+        <v>480.42</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>8.9915777653003932</v>
+      </c>
+      <c r="E6">
+        <v>468.59</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8.7701665730862803</v>
+      </c>
+      <c r="G6">
+        <v>493.47</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>9.2358225715889954</v>
+      </c>
+      <c r="I6">
+        <v>562.72</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>10.531910911472956</v>
+      </c>
+      <c r="K6">
+        <v>477.75</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>8.9416058394160576</v>
+      </c>
+      <c r="M6">
+        <v>468.68</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>8.7718510200262028</v>
+      </c>
+      <c r="O6">
+        <v>902.9</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>16.898746022833613</v>
+      </c>
+      <c r="Q6">
+        <v>967232</v>
+      </c>
+      <c r="R6">
+        <v>1133240</v>
+      </c>
+      <c r="S6">
+        <v>1023756</v>
+      </c>
+      <c r="T6">
+        <v>916832</v>
+      </c>
+      <c r="U6">
+        <v>987972</v>
+      </c>
+      <c r="V6">
+        <v>1133440</v>
+      </c>
+      <c r="W6">
+        <v>962568</v>
+      </c>
+      <c r="X6">
+        <v>1358792</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>12.6</v>
+      </c>
+      <c r="C7">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5.3777777777777782</v>
+      </c>
+      <c r="E7">
+        <v>69.61</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>5.5246031746031745</v>
+      </c>
+      <c r="G7">
+        <v>64.98</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>5.1571428571428575</v>
+      </c>
+      <c r="I7">
+        <v>525.98</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>41.744444444444447</v>
+      </c>
+      <c r="K7">
+        <v>78.63</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>6.2404761904761905</v>
+      </c>
+      <c r="M7">
+        <v>68.64</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>5.4476190476190478</v>
+      </c>
+      <c r="O7">
+        <v>236.64</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>18.780952380952382</v>
+      </c>
+      <c r="Q7">
+        <v>1508668</v>
+      </c>
+      <c r="R7">
+        <v>2081952</v>
+      </c>
+      <c r="S7">
+        <v>2419564</v>
+      </c>
+      <c r="T7">
+        <v>1053756</v>
+      </c>
+      <c r="U7">
+        <v>1485980</v>
+      </c>
+      <c r="V7">
+        <v>2061748</v>
+      </c>
+      <c r="W7">
+        <v>1931000</v>
+      </c>
+      <c r="X7">
+        <v>2405512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>82.32</v>
+      </c>
+      <c r="C8">
+        <v>175.15</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.1276724975704568</v>
+      </c>
+      <c r="E8">
+        <v>177.19</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2.1524538386783285</v>
+      </c>
+      <c r="G8">
+        <v>182.27</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>2.2141642371234211</v>
+      </c>
+      <c r="I8">
+        <v>189.17</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>2.2979834791059282</v>
+      </c>
+      <c r="K8">
+        <v>174.18</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>2.1158892128279887</v>
+      </c>
+      <c r="M8">
+        <v>194.36</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>2.361030126336249</v>
+      </c>
+      <c r="O8">
+        <v>252.89</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>3.0720359572400389</v>
+      </c>
+      <c r="Q8">
+        <v>2495116</v>
+      </c>
+      <c r="R8">
+        <v>2871740</v>
+      </c>
+      <c r="S8">
+        <v>3934060</v>
+      </c>
+      <c r="T8">
+        <v>3014620</v>
+      </c>
+      <c r="U8">
+        <v>2960676</v>
+      </c>
+      <c r="V8">
+        <v>2873764</v>
+      </c>
+      <c r="W8">
+        <v>3281704</v>
+      </c>
+      <c r="X8">
+        <v>3978984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9">
+        <v>4.72</v>
+      </c>
+      <c r="C9">
+        <v>7.44</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.5762711864406782</v>
+      </c>
+      <c r="E9">
+        <v>7.57</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.603813559322034</v>
+      </c>
+      <c r="G9">
+        <v>7.74</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>1.6398305084745763</v>
+      </c>
+      <c r="I9">
+        <v>8.25</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>1.7478813559322035</v>
+      </c>
+      <c r="K9">
+        <v>7.52</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>1.5932203389830508</v>
+      </c>
+      <c r="M9">
+        <v>7.96</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>1.6864406779661019</v>
+      </c>
+      <c r="O9">
+        <v>9.23</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>1.9555084745762714</v>
+      </c>
+      <c r="Q9">
+        <v>68468</v>
+      </c>
+      <c r="R9">
+        <v>128744</v>
+      </c>
+      <c r="S9">
+        <v>361832</v>
+      </c>
+      <c r="T9">
+        <v>130032</v>
+      </c>
+      <c r="U9">
+        <v>129652</v>
+      </c>
+      <c r="V9">
+        <v>130296</v>
+      </c>
+      <c r="W9">
+        <v>164232</v>
+      </c>
+      <c r="X9">
+        <v>155280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>29.76</v>
+      </c>
+      <c r="C10">
+        <v>41.3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.387768817204301</v>
+      </c>
+      <c r="E10">
+        <v>42.29</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1.421034946236559</v>
+      </c>
+      <c r="G10">
+        <v>41.86</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>1.4065860215053763</v>
+      </c>
+      <c r="I10">
+        <v>41.32</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>1.3884408602150538</v>
+      </c>
+      <c r="K10">
+        <v>42.28</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>1.4206989247311828</v>
+      </c>
+      <c r="M10">
+        <v>43.14</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>1.4495967741935483</v>
+      </c>
+      <c r="O10">
+        <v>44.1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>1.4818548387096775</v>
+      </c>
+      <c r="Q10">
+        <v>417768</v>
+      </c>
+      <c r="R10">
+        <v>519064</v>
+      </c>
+      <c r="S10">
+        <v>588084</v>
+      </c>
+      <c r="T10">
+        <v>512192</v>
+      </c>
+      <c r="U10">
+        <v>539560</v>
+      </c>
+      <c r="V10">
+        <v>520824</v>
+      </c>
+      <c r="W10">
+        <v>555848</v>
+      </c>
+      <c r="X10">
+        <v>575424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>69.88</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.5881818181818181</v>
+      </c>
+      <c r="E11">
+        <v>74.150000000000006</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1.6852272727272728</v>
+      </c>
+      <c r="G11">
+        <v>72.14</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>1.6395454545454546</v>
+      </c>
+      <c r="I11">
+        <v>70.59</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>1.604318181818182</v>
+      </c>
+      <c r="K11">
+        <v>70.2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>1.5954545454545455</v>
+      </c>
+      <c r="M11">
+        <v>73.61</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>1.6729545454545454</v>
+      </c>
+      <c r="O11">
+        <v>628.19000000000005</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>14.277045454545457</v>
+      </c>
+      <c r="Q11">
+        <v>2525896</v>
+      </c>
+      <c r="R11">
+        <v>2965116</v>
+      </c>
+      <c r="S11">
+        <v>3103888</v>
+      </c>
+      <c r="T11">
+        <v>2247020</v>
+      </c>
+      <c r="U11">
+        <v>2181540</v>
+      </c>
+      <c r="V11">
+        <v>2414916</v>
+      </c>
+      <c r="W11">
+        <v>3600116</v>
+      </c>
+      <c r="X11">
+        <v>2062376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>1.89</v>
+      </c>
+      <c r="C12">
+        <v>2.6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.3756613756613758</v>
+      </c>
+      <c r="E12">
+        <v>2.33</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>1.232804232804233</v>
+      </c>
+      <c r="G12">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="I12">
+        <v>2.39</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>1.2645502645502646</v>
+      </c>
+      <c r="K12">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>1.2962962962962965</v>
+      </c>
+      <c r="M12">
+        <v>2.58</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>1.3650793650793651</v>
+      </c>
+      <c r="O12">
+        <v>2.5</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>1.3227513227513228</v>
+      </c>
+      <c r="Q12">
+        <v>245192</v>
+      </c>
+      <c r="R12">
+        <v>351252</v>
+      </c>
+      <c r="S12">
+        <v>419504</v>
+      </c>
+      <c r="T12">
+        <v>367764</v>
+      </c>
+      <c r="U12">
+        <v>352768</v>
+      </c>
+      <c r="V12">
+        <v>350168</v>
+      </c>
+      <c r="W12">
+        <v>440200</v>
+      </c>
+      <c r="X12">
+        <v>353760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>53.53</v>
+      </c>
+      <c r="C13">
+        <v>53.99</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.0085933121614048</v>
+      </c>
+      <c r="E13">
+        <v>55.22</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>1.0315710816364654</v>
+      </c>
+      <c r="G13">
+        <v>54.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>1.0181206799925275</v>
+      </c>
+      <c r="I13">
+        <v>55.01</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>1.0276480478236503</v>
+      </c>
+      <c r="K13">
+        <v>55.88</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>1.0439006164767421</v>
+      </c>
+      <c r="M13">
+        <v>53.93</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>1.0074724453577433</v>
+      </c>
+      <c r="O13">
+        <v>54.18</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>1.012142723706333</v>
+      </c>
+      <c r="Q13">
+        <v>844712</v>
+      </c>
+      <c r="R13">
+        <v>864292</v>
+      </c>
+      <c r="S13">
+        <v>891144</v>
+      </c>
+      <c r="T13">
+        <v>863160</v>
+      </c>
+      <c r="U13">
+        <v>860192</v>
+      </c>
+      <c r="V13">
+        <v>862940</v>
+      </c>
+      <c r="W13">
+        <v>869724</v>
+      </c>
+      <c r="X13">
+        <v>857508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <v>89.78</v>
+      </c>
+      <c r="C14">
+        <v>775.68</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>8.6397861439073278</v>
+      </c>
+      <c r="E14">
+        <v>777.46</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>8.659612385832034</v>
+      </c>
+      <c r="G14">
+        <v>847.68</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>9.4417464914234781</v>
+      </c>
+      <c r="I14">
+        <v>891.82</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>9.9333927378035209</v>
+      </c>
+      <c r="K14">
+        <v>775.13</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>8.633660057919359</v>
+      </c>
+      <c r="M14">
+        <v>778.76</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>8.6740922254399635</v>
+      </c>
+      <c r="O14">
+        <v>1052.46</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="6"/>
+        <v>11.722655379817331</v>
+      </c>
+      <c r="Q14">
+        <v>1161184</v>
+      </c>
+      <c r="R14">
+        <v>1412792</v>
+      </c>
+      <c r="S14">
+        <v>1912952</v>
+      </c>
+      <c r="T14">
+        <v>1365684</v>
+      </c>
+      <c r="U14">
+        <v>1396044</v>
+      </c>
+      <c r="V14">
+        <v>1413956</v>
+      </c>
+      <c r="W14">
+        <v>2013840</v>
+      </c>
+      <c r="X14">
+        <v>2054448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15">
+        <v>67.41</v>
+      </c>
+      <c r="C15">
+        <v>73.790000000000006</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.0946447114671416</v>
+      </c>
+      <c r="E15">
+        <v>74.36</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1.1031004302032339</v>
+      </c>
+      <c r="G15">
+        <v>71.319999999999993</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>1.0580032636107402</v>
+      </c>
+      <c r="I15">
+        <v>73.25</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>1.0866340305592643</v>
+      </c>
+      <c r="K15">
+        <v>72.81</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>1.0801068090787718</v>
+      </c>
+      <c r="M15">
+        <v>74.95</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>1.1118528408248036</v>
+      </c>
+      <c r="O15">
+        <v>72.8</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="6"/>
+        <v>1.0799584631360333</v>
+      </c>
+      <c r="Q15">
+        <v>115852</v>
+      </c>
+      <c r="R15">
+        <v>343464</v>
+      </c>
+      <c r="S15">
+        <v>364988</v>
+      </c>
+      <c r="T15">
+        <v>175424</v>
+      </c>
+      <c r="U15">
+        <v>171856</v>
+      </c>
+      <c r="V15">
+        <v>336376</v>
+      </c>
+      <c r="W15">
+        <v>229104</v>
+      </c>
+      <c r="X15">
+        <v>172664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="C16">
+        <v>141.41</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>3.8270635994587274</v>
+      </c>
+      <c r="E16">
+        <v>190.13</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5.145602165087956</v>
+      </c>
+      <c r="G16">
+        <v>165.47</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>4.4782138024357234</v>
+      </c>
+      <c r="I16">
+        <v>397.46</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>10.756698240866033</v>
+      </c>
+      <c r="K16">
+        <v>238.99</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>6.4679296346414068</v>
+      </c>
+      <c r="M16">
+        <v>174.12</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>4.7123139377537209</v>
+      </c>
+      <c r="O16">
+        <v>1230.3399999999999</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>33.29742895805142</v>
+      </c>
+      <c r="Q16">
+        <v>8608</v>
+      </c>
+      <c r="R16">
+        <v>53464</v>
+      </c>
+      <c r="S16">
+        <v>250668</v>
+      </c>
+      <c r="T16">
+        <v>55040</v>
+      </c>
+      <c r="U16">
+        <v>49396</v>
+      </c>
+      <c r="V16">
+        <v>51512</v>
+      </c>
+      <c r="W16">
+        <v>84284</v>
+      </c>
+      <c r="X16">
+        <v>52040</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17">
+        <v>116.79</v>
+      </c>
+      <c r="C17">
+        <v>313.12</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.6810514598852642</v>
+      </c>
+      <c r="E17">
+        <v>313.70999999999998</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>2.6861032622656045</v>
+      </c>
+      <c r="G17">
+        <v>295.43</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>2.5295830122441991</v>
+      </c>
+      <c r="I17">
+        <v>279.43</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>2.3925849815908897</v>
+      </c>
+      <c r="K17">
+        <v>312.57</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>2.6763421525815563</v>
+      </c>
+      <c r="M17">
+        <v>306.41000000000003</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>2.6235979107800325</v>
+      </c>
+      <c r="O17">
+        <v>322.93</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
+        <v>2.7650483774295744</v>
+      </c>
+      <c r="Q17">
+        <v>31548</v>
+      </c>
+      <c r="R17">
+        <v>50344</v>
+      </c>
+      <c r="S17">
+        <v>79232</v>
+      </c>
+      <c r="T17">
+        <v>52752</v>
+      </c>
+      <c r="U17">
+        <v>62408</v>
+      </c>
+      <c r="V17">
+        <v>49216</v>
+      </c>
+      <c r="W17">
+        <v>48996</v>
+      </c>
+      <c r="X17">
+        <v>76096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>52.74</v>
+      </c>
+      <c r="C18">
+        <v>66.790000000000006</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.2664012135001896</v>
+      </c>
+      <c r="E18">
+        <v>66.81</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>1.2667804323094425</v>
+      </c>
+      <c r="G18">
+        <v>66.819999999999993</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>1.2669700417140688</v>
+      </c>
+      <c r="I18">
+        <v>66.17</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>1.2546454304133485</v>
+      </c>
+      <c r="K18">
+        <v>66.540000000000006</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>1.2616609783845278</v>
+      </c>
+      <c r="M18">
+        <v>65.91</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>1.2497155858930602</v>
+      </c>
+      <c r="O18">
+        <v>66.64</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>1.2635570724307925</v>
+      </c>
+      <c r="Q18">
+        <v>496328</v>
+      </c>
+      <c r="R18">
+        <v>854632</v>
+      </c>
+      <c r="S18">
+        <v>1662308</v>
+      </c>
+      <c r="T18">
+        <v>969468</v>
+      </c>
+      <c r="U18">
+        <v>915092</v>
+      </c>
+      <c r="V18">
+        <v>843284</v>
+      </c>
+      <c r="W18">
+        <v>1048964</v>
+      </c>
+      <c r="X18">
+        <v>950592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>AVERAGE(B4:B18)</f>
+        <v>49.301333333333332</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:O19" si="7">AVERAGE(C4:C18)</f>
+        <v>159.61000000000001</v>
+      </c>
+      <c r="D19">
+        <f>AVERAGE(D4:D18)</f>
+        <v>2.9166132044655511</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="7"/>
+        <v>162.92799999999997</v>
+      </c>
+      <c r="F19">
+        <f>AVERAGE(F4:F18)</f>
+        <v>3.0054373615495269</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="7"/>
+        <v>166.02199999999999</v>
+      </c>
+      <c r="H19">
+        <f>AVERAGE(H4:H18)</f>
+        <v>3.0108951759660334</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>219.45933333333332</v>
+      </c>
+      <c r="J19">
+        <f>AVERAGE(J4:J18)</f>
+        <v>5.9958208521882792</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="7"/>
+        <v>166.73533333333336</v>
+      </c>
+      <c r="L19">
+        <f>AVERAGE(L4:L18)</f>
+        <v>3.1473722591707083</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>162.51733333333331</v>
+      </c>
+      <c r="N19">
+        <f>AVERAGE(N4:N18)</f>
+        <v>2.9957046900597746</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>333.83866666666671</v>
+      </c>
+      <c r="P19">
+        <f>AVERAGE(P4:P18)</f>
+        <v>7.4616960338396439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q2:X2"/>
+    <mergeCell ref="B2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6399,11 +7942,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -6693,7 +8236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
@@ -8734,7 +10277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
@@ -9829,7 +11372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
@@ -11234,7 +12777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
@@ -11567,7 +13110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrected error in data on new "mmprof new experimental" sheet
</commit_message>
<xml_diff>
--- a/paper/data4.xlsx
+++ b/paper/data4.xlsx
@@ -26,7 +26,7 @@
     <definedName name="data" localSheetId="0">Baseline!$A$1:$M$17</definedName>
     <definedName name="data" localSheetId="4">Explaination!$A$1:$M$17</definedName>
     <definedName name="data" localSheetId="2">mmprof!$A$1:$L$17</definedName>
-    <definedName name="data" localSheetId="1">'mmprof new experimental'!$A$2:$Y$18</definedName>
+    <definedName name="data" localSheetId="1">'mmprof new experimental'!$A$2:$AF$18</definedName>
     <definedName name="data" localSheetId="8">Sheet8!$A$1:$R$17</definedName>
     <definedName name="data_1" localSheetId="0">Baseline!$A$23:$M$39</definedName>
     <definedName name="data_1" localSheetId="4">Explaination!$A$23:$M$39</definedName>
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="117">
   <si>
     <t>benchmark</t>
   </si>
@@ -720,7 +720,25 @@
     <t>SRG1, 2019-07-19 12:15:30, 10 runs, maprof</t>
   </si>
   <si>
-    <t>x</t>
+    <t>hoard-mmprof</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cmalloc224-mmprof </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   tcmalloc -mmprof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    omalloc -mmprof</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cmalloc221 -mmprof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   jemalloc -mmprof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  dieharder -mmprof</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1503,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1510,6 +1528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="655">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2539,7 +2558,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4580,44 +4599,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.83203125" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.83203125" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.1640625" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" customWidth="1"/>
+    <col min="24" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>82</v>
       </c>
@@ -4637,19 +4658,26 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15" t="s">
-        <v>107</v>
-      </c>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
       <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W2" s="14"/>
+      <c r="X2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>83</v>
       </c>
@@ -4659,1335 +4687,1694 @@
       <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" t="s">
+        <v>115</v>
+      </c>
+      <c r="U3" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" t="s">
+        <v>116</v>
+      </c>
+      <c r="X3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z3" t="s">
         <v>86</v>
       </c>
-      <c r="G3" t="s">
+      <c r="AA3" t="s">
         <v>87</v>
       </c>
-      <c r="I3" t="s">
+      <c r="AB3" t="s">
         <v>88</v>
       </c>
-      <c r="K3" t="s">
+      <c r="AC3" t="s">
         <v>89</v>
       </c>
-      <c r="M3" t="s">
+      <c r="AD3" t="s">
         <v>90</v>
       </c>
-      <c r="O3" t="s">
+      <c r="AE3" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" t="s">
-        <v>85</v>
-      </c>
-      <c r="R3" t="s">
-        <v>84</v>
-      </c>
-      <c r="S3" t="s">
-        <v>86</v>
-      </c>
-      <c r="T3" t="s">
-        <v>87</v>
-      </c>
-      <c r="U3" t="s">
-        <v>88</v>
-      </c>
-      <c r="V3" t="s">
-        <v>89</v>
-      </c>
-      <c r="W3" t="s">
-        <v>90</v>
-      </c>
-      <c r="X3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>92</v>
       </c>
       <c r="B4">
         <v>58.3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
+        <v>60.89</v>
+      </c>
+      <c r="D4" s="8">
         <v>65.25</v>
       </c>
-      <c r="D4">
-        <f>C4/$B4</f>
-        <v>1.1192109777015438</v>
-      </c>
-      <c r="E4">
+      <c r="E4" s="8">
+        <f>D4/C4</f>
+        <v>1.0716045327640007</v>
+      </c>
+      <c r="F4" s="8">
+        <v>60.52</v>
+      </c>
+      <c r="G4" s="8">
         <v>65.16</v>
       </c>
-      <c r="F4">
-        <f>E4/$B4</f>
-        <v>1.1176672384219555</v>
-      </c>
-      <c r="G4">
+      <c r="H4" s="8">
+        <f>G4/F4</f>
+        <v>1.076668869795109</v>
+      </c>
+      <c r="I4" s="8">
+        <v>60.85</v>
+      </c>
+      <c r="J4" s="8">
         <v>65.05</v>
       </c>
-      <c r="H4">
-        <f>G4/$B4</f>
-        <v>1.1157804459691252</v>
-      </c>
-      <c r="I4">
+      <c r="K4" s="8">
+        <f>J4/I4</f>
+        <v>1.0690221857025473</v>
+      </c>
+      <c r="L4" s="8">
+        <v>61.35</v>
+      </c>
+      <c r="M4" s="8">
         <v>65.25</v>
       </c>
-      <c r="J4">
-        <f>I4/$B4</f>
-        <v>1.1192109777015438</v>
-      </c>
-      <c r="K4">
+      <c r="N4" s="8">
+        <f>M4/L4</f>
+        <v>1.0635696821515892</v>
+      </c>
+      <c r="O4" s="8">
+        <v>60.58</v>
+      </c>
+      <c r="P4" s="8">
         <v>65.22</v>
       </c>
-      <c r="L4">
-        <f>K4/$B4</f>
-        <v>1.1186963979416811</v>
-      </c>
-      <c r="M4">
+      <c r="Q4" s="8">
+        <f>P4/O4</f>
+        <v>1.0765929349620338</v>
+      </c>
+      <c r="R4" s="8">
+        <v>61.2</v>
+      </c>
+      <c r="S4" s="8">
         <v>65.400000000000006</v>
       </c>
-      <c r="N4">
-        <f>M4/$B4</f>
-        <v>1.1217838765008579</v>
-      </c>
-      <c r="O4">
+      <c r="T4" s="8">
+        <f>S4/R4</f>
+        <v>1.0686274509803921</v>
+      </c>
+      <c r="U4" s="8">
+        <v>61.19</v>
+      </c>
+      <c r="V4" s="8">
         <v>65.98</v>
       </c>
-      <c r="P4">
-        <f>O4/$B4</f>
-        <v>1.1317324185248714</v>
-      </c>
-      <c r="Q4">
+      <c r="W4">
+        <f>V4/U4</f>
+        <v>1.0782807648308548</v>
+      </c>
+      <c r="X4">
         <v>627176</v>
       </c>
-      <c r="R4">
+      <c r="Y4">
         <v>754552</v>
       </c>
-      <c r="S4">
+      <c r="Z4">
         <v>801496</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <v>751640</v>
       </c>
-      <c r="U4">
+      <c r="AB4">
         <v>744096</v>
       </c>
-      <c r="V4">
+      <c r="AC4">
         <v>756728</v>
       </c>
-      <c r="W4">
+      <c r="AD4">
         <v>784656</v>
       </c>
-      <c r="X4">
+      <c r="AE4">
         <v>753300</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B5">
         <v>35.299999999999997</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
+        <v>31.67</v>
+      </c>
+      <c r="D5" s="8">
         <v>59.57</v>
       </c>
-      <c r="D5">
-        <f t="shared" ref="D5:D18" si="0">C5/$B5</f>
-        <v>1.6875354107648726</v>
-      </c>
-      <c r="E5">
+      <c r="E5" s="8">
+        <f t="shared" ref="E5:E18" si="0">D5/C5</f>
+        <v>1.8809598989580043</v>
+      </c>
+      <c r="F5" s="8">
+        <v>31.54</v>
+      </c>
+      <c r="G5" s="8">
         <v>59.34</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F18" si="1">E5/$B5</f>
-        <v>1.6810198300283288</v>
-      </c>
-      <c r="G5">
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:H18" si="1">G5/F5</f>
+        <v>1.88142041851617</v>
+      </c>
+      <c r="I5" s="8">
+        <v>31.9</v>
+      </c>
+      <c r="J5" s="8">
         <v>59.17</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H18" si="2">G5/$B5</f>
-        <v>1.676203966005666</v>
-      </c>
-      <c r="I5">
+      <c r="K5" s="8">
+        <f t="shared" ref="K5:K18" si="2">J5/I5</f>
+        <v>1.8548589341692792</v>
+      </c>
+      <c r="L5" s="8">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="M5" s="8">
         <v>63.08</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J18" si="3">I5/$B5</f>
-        <v>1.7869688385269122</v>
-      </c>
-      <c r="K5">
+      <c r="N5" s="8">
+        <f t="shared" ref="N5:N18" si="3">M5/L5</f>
+        <v>1.8903206472879832</v>
+      </c>
+      <c r="O5" s="8">
+        <v>31.69</v>
+      </c>
+      <c r="P5" s="8">
         <v>60.88</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L18" si="4">K5/$B5</f>
-        <v>1.7246458923512751</v>
-      </c>
-      <c r="M5">
+      <c r="Q5" s="8">
+        <f t="shared" ref="Q5:Q18" si="4">P5/O5</f>
+        <v>1.9211107604922688</v>
+      </c>
+      <c r="R5" s="8">
+        <v>31.46</v>
+      </c>
+      <c r="S5" s="8">
         <v>59.31</v>
       </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N18" si="5">M5/$B5</f>
-        <v>1.6801699716713883</v>
-      </c>
-      <c r="O5">
+      <c r="T5" s="8">
+        <f t="shared" ref="T5:T18" si="5">S5/R5</f>
+        <v>1.8852511125238398</v>
+      </c>
+      <c r="U5" s="8">
+        <v>34</v>
+      </c>
+      <c r="V5" s="8">
         <v>65.8</v>
       </c>
-      <c r="P5">
-        <f t="shared" ref="P5:P18" si="6">O5/$B5</f>
-        <v>1.8640226628895185</v>
-      </c>
-      <c r="Q5">
+      <c r="W5">
+        <f t="shared" ref="W5:W18" si="6">V5/U5</f>
+        <v>1.9352941176470588</v>
+      </c>
+      <c r="X5">
         <v>34188</v>
       </c>
-      <c r="R5">
+      <c r="Y5">
         <v>87576</v>
       </c>
-      <c r="S5">
+      <c r="Z5">
         <v>247392</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <v>90116</v>
       </c>
-      <c r="U5">
+      <c r="AB5">
         <v>82760</v>
       </c>
-      <c r="V5">
+      <c r="AC5">
         <v>92156</v>
       </c>
-      <c r="W5">
+      <c r="AD5">
         <v>104420</v>
       </c>
-      <c r="X5">
+      <c r="AE5">
         <v>90496</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B6">
         <v>53.43</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
+        <v>61.48</v>
+      </c>
+      <c r="D6" s="8">
         <v>480.42</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
-        <v>8.9915777653003932</v>
-      </c>
-      <c r="E6">
+        <v>7.8142485361093046</v>
+      </c>
+      <c r="F6" s="8">
+        <v>57.03</v>
+      </c>
+      <c r="G6" s="8">
         <v>468.59</v>
       </c>
-      <c r="F6">
+      <c r="H6" s="8">
         <f t="shared" si="1"/>
-        <v>8.7701665730862803</v>
-      </c>
-      <c r="G6">
+        <v>8.2165526915658411</v>
+      </c>
+      <c r="I6" s="8">
+        <v>57.54</v>
+      </c>
+      <c r="J6" s="8">
         <v>493.47</v>
       </c>
-      <c r="H6">
+      <c r="K6" s="8">
         <f t="shared" si="2"/>
-        <v>9.2358225715889954</v>
-      </c>
-      <c r="I6">
+        <v>8.5761209593326395</v>
+      </c>
+      <c r="L6" s="8">
+        <v>67.150000000000006</v>
+      </c>
+      <c r="M6" s="8">
         <v>562.72</v>
       </c>
-      <c r="J6">
+      <c r="N6" s="8">
         <f t="shared" si="3"/>
-        <v>10.531910911472956</v>
-      </c>
-      <c r="K6">
+        <v>8.3800446760982865</v>
+      </c>
+      <c r="O6" s="8">
+        <v>61.52</v>
+      </c>
+      <c r="P6" s="8">
         <v>477.75</v>
       </c>
-      <c r="L6">
+      <c r="Q6" s="8">
         <f t="shared" si="4"/>
-        <v>8.9416058394160576</v>
-      </c>
-      <c r="M6">
+        <v>7.7657672301690504</v>
+      </c>
+      <c r="R6" s="8">
+        <v>60.39</v>
+      </c>
+      <c r="S6" s="8">
         <v>468.68</v>
       </c>
-      <c r="N6">
+      <c r="T6" s="8">
         <f t="shared" si="5"/>
-        <v>8.7718510200262028</v>
-      </c>
-      <c r="O6">
+        <v>7.7608875641662527</v>
+      </c>
+      <c r="U6" s="8">
+        <v>92.84</v>
+      </c>
+      <c r="V6" s="8">
         <v>902.9</v>
       </c>
-      <c r="P6">
+      <c r="W6">
         <f t="shared" si="6"/>
-        <v>16.898746022833613</v>
-      </c>
-      <c r="Q6">
+        <v>9.7253339077983618</v>
+      </c>
+      <c r="X6">
         <v>967232</v>
       </c>
-      <c r="R6">
+      <c r="Y6">
         <v>1133240</v>
       </c>
-      <c r="S6">
+      <c r="Z6">
         <v>1023756</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <v>916832</v>
       </c>
-      <c r="U6">
+      <c r="AB6">
         <v>987972</v>
       </c>
-      <c r="V6">
+      <c r="AC6">
         <v>1133440</v>
       </c>
-      <c r="W6">
+      <c r="AD6">
         <v>962568</v>
       </c>
-      <c r="X6">
+      <c r="AE6">
         <v>1358792</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>95</v>
       </c>
       <c r="B7">
         <v>12.6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
+        <v>12.67</v>
+      </c>
+      <c r="D7" s="8">
         <v>67.760000000000005</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>5.3777777777777782</v>
-      </c>
-      <c r="E7">
+        <v>5.348066298342542</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10.23</v>
+      </c>
+      <c r="G7" s="8">
         <v>69.61</v>
       </c>
-      <c r="F7">
+      <c r="H7" s="8">
         <f t="shared" si="1"/>
-        <v>5.5246031746031745</v>
-      </c>
-      <c r="G7">
+        <v>6.8044965786901264</v>
+      </c>
+      <c r="I7" s="8">
+        <v>10.58</v>
+      </c>
+      <c r="J7" s="8">
         <v>64.98</v>
       </c>
-      <c r="H7">
+      <c r="K7" s="8">
         <f t="shared" si="2"/>
-        <v>5.1571428571428575</v>
-      </c>
-      <c r="I7">
+        <v>6.1417769376181477</v>
+      </c>
+      <c r="L7" s="8">
+        <v>23.35</v>
+      </c>
+      <c r="M7" s="8">
         <v>525.98</v>
       </c>
-      <c r="J7">
+      <c r="N7" s="8">
         <f t="shared" si="3"/>
-        <v>41.744444444444447</v>
-      </c>
-      <c r="K7">
+        <v>22.525910064239827</v>
+      </c>
+      <c r="O7" s="8">
+        <v>16.53</v>
+      </c>
+      <c r="P7" s="8">
         <v>78.63</v>
       </c>
-      <c r="L7">
+      <c r="Q7" s="8">
         <f t="shared" si="4"/>
-        <v>6.2404761904761905</v>
-      </c>
-      <c r="M7">
+        <v>4.7568058076225039</v>
+      </c>
+      <c r="R7" s="8">
+        <v>10.39</v>
+      </c>
+      <c r="S7" s="8">
         <v>68.64</v>
       </c>
-      <c r="N7">
+      <c r="T7" s="8">
         <f t="shared" si="5"/>
-        <v>5.4476190476190478</v>
-      </c>
-      <c r="O7">
+        <v>6.6063522617901826</v>
+      </c>
+      <c r="U7" s="8">
+        <v>27.64</v>
+      </c>
+      <c r="V7" s="8">
         <v>236.64</v>
       </c>
-      <c r="P7">
+      <c r="W7">
         <f t="shared" si="6"/>
-        <v>18.780952380952382</v>
-      </c>
-      <c r="Q7">
+        <v>8.5615050651230096</v>
+      </c>
+      <c r="X7">
         <v>1508668</v>
       </c>
-      <c r="R7">
+      <c r="Y7">
         <v>2081952</v>
       </c>
-      <c r="S7">
+      <c r="Z7">
         <v>2419564</v>
       </c>
-      <c r="T7">
+      <c r="AA7">
         <v>1053756</v>
       </c>
-      <c r="U7">
+      <c r="AB7">
         <v>1485980</v>
       </c>
-      <c r="V7">
+      <c r="AC7">
         <v>2061748</v>
       </c>
-      <c r="W7">
+      <c r="AD7">
         <v>1931000</v>
       </c>
-      <c r="X7">
+      <c r="AE7">
         <v>2405512</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>96</v>
       </c>
       <c r="B8">
         <v>82.32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
+        <v>89.2</v>
+      </c>
+      <c r="D8" s="8">
         <v>175.15</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
-        <v>2.1276724975704568</v>
-      </c>
-      <c r="E8">
+        <v>1.9635650224215246</v>
+      </c>
+      <c r="F8" s="8">
+        <v>90.21</v>
+      </c>
+      <c r="G8" s="8">
         <v>177.19</v>
       </c>
-      <c r="F8">
+      <c r="H8" s="8">
         <f t="shared" si="1"/>
-        <v>2.1524538386783285</v>
-      </c>
-      <c r="G8">
+        <v>1.9641946569116506</v>
+      </c>
+      <c r="I8" s="8">
+        <v>91.12</v>
+      </c>
+      <c r="J8" s="8">
         <v>182.27</v>
       </c>
-      <c r="H8">
+      <c r="K8" s="8">
         <f t="shared" si="2"/>
-        <v>2.2141642371234211</v>
-      </c>
-      <c r="I8">
+        <v>2.0003292361720808</v>
+      </c>
+      <c r="L8" s="8">
+        <v>91.05</v>
+      </c>
+      <c r="M8" s="8">
         <v>189.17</v>
       </c>
-      <c r="J8">
+      <c r="N8" s="8">
         <f t="shared" si="3"/>
-        <v>2.2979834791059282</v>
-      </c>
-      <c r="K8">
+        <v>2.0776496430532672</v>
+      </c>
+      <c r="O8" s="8">
+        <v>88.59</v>
+      </c>
+      <c r="P8" s="8">
         <v>174.18</v>
       </c>
-      <c r="L8">
+      <c r="Q8" s="8">
         <f t="shared" si="4"/>
-        <v>2.1158892128279887</v>
-      </c>
-      <c r="M8">
+        <v>1.9661361327463596</v>
+      </c>
+      <c r="R8" s="8">
+        <v>87.73</v>
+      </c>
+      <c r="S8" s="8">
         <v>194.36</v>
       </c>
-      <c r="N8">
+      <c r="T8" s="8">
         <f t="shared" si="5"/>
-        <v>2.361030126336249</v>
-      </c>
-      <c r="O8">
+        <v>2.2154337170865155</v>
+      </c>
+      <c r="U8" s="8">
+        <v>101.41</v>
+      </c>
+      <c r="V8" s="8">
         <v>252.89</v>
       </c>
-      <c r="P8">
+      <c r="W8">
         <f t="shared" si="6"/>
-        <v>3.0720359572400389</v>
-      </c>
-      <c r="Q8">
+        <v>2.4937382901094565</v>
+      </c>
+      <c r="X8">
         <v>2495116</v>
       </c>
-      <c r="R8">
+      <c r="Y8">
         <v>2871740</v>
       </c>
-      <c r="S8">
+      <c r="Z8">
         <v>3934060</v>
       </c>
-      <c r="T8">
+      <c r="AA8">
         <v>3014620</v>
       </c>
-      <c r="U8">
+      <c r="AB8">
         <v>2960676</v>
       </c>
-      <c r="V8">
+      <c r="AC8">
         <v>2873764</v>
       </c>
-      <c r="W8">
+      <c r="AD8">
         <v>3281704</v>
       </c>
-      <c r="X8">
+      <c r="AE8">
         <v>3978984</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>97</v>
       </c>
       <c r="B9">
         <v>4.72</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="D9" s="8">
         <v>7.44</v>
       </c>
-      <c r="D9">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
-        <v>1.5762711864406782</v>
-      </c>
-      <c r="E9">
+        <v>1.5829787234042554</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4.72</v>
+      </c>
+      <c r="G9" s="8">
         <v>7.57</v>
       </c>
-      <c r="F9">
+      <c r="H9" s="8">
         <f t="shared" si="1"/>
         <v>1.603813559322034</v>
       </c>
-      <c r="G9">
+      <c r="I9" s="8">
+        <v>4.71</v>
+      </c>
+      <c r="J9" s="8">
         <v>7.74</v>
       </c>
-      <c r="H9">
+      <c r="K9" s="8">
         <f t="shared" si="2"/>
-        <v>1.6398305084745763</v>
-      </c>
-      <c r="I9">
+        <v>1.6433121019108281</v>
+      </c>
+      <c r="L9" s="8">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="M9" s="8">
         <v>8.25</v>
       </c>
-      <c r="J9">
+      <c r="N9" s="8">
         <f t="shared" si="3"/>
-        <v>1.7478813559322035</v>
-      </c>
-      <c r="K9">
+        <v>1.7441860465116277</v>
+      </c>
+      <c r="O9" s="8">
+        <v>4.68</v>
+      </c>
+      <c r="P9" s="8">
         <v>7.52</v>
       </c>
-      <c r="L9">
+      <c r="Q9" s="8">
         <f t="shared" si="4"/>
-        <v>1.5932203389830508</v>
-      </c>
-      <c r="M9">
+        <v>1.6068376068376069</v>
+      </c>
+      <c r="R9" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="S9" s="8">
         <v>7.96</v>
       </c>
-      <c r="N9">
+      <c r="T9" s="8">
         <f t="shared" si="5"/>
-        <v>1.6864406779661019</v>
-      </c>
-      <c r="O9">
+        <v>1.6936170212765957</v>
+      </c>
+      <c r="U9" s="8">
+        <v>4.83</v>
+      </c>
+      <c r="V9" s="8">
         <v>9.23</v>
       </c>
-      <c r="P9">
+      <c r="W9">
         <f t="shared" si="6"/>
-        <v>1.9555084745762714</v>
-      </c>
-      <c r="Q9">
+        <v>1.9109730848861284</v>
+      </c>
+      <c r="X9">
         <v>68468</v>
       </c>
-      <c r="R9">
+      <c r="Y9">
         <v>128744</v>
       </c>
-      <c r="S9">
+      <c r="Z9">
         <v>361832</v>
       </c>
-      <c r="T9">
+      <c r="AA9">
         <v>130032</v>
       </c>
-      <c r="U9">
+      <c r="AB9">
         <v>129652</v>
       </c>
-      <c r="V9">
+      <c r="AC9">
         <v>130296</v>
       </c>
-      <c r="W9">
+      <c r="AD9">
         <v>164232</v>
       </c>
-      <c r="X9">
+      <c r="AE9">
         <v>155280</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>98</v>
       </c>
       <c r="B10">
         <v>29.76</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
+        <v>39.86</v>
+      </c>
+      <c r="D10" s="8">
         <v>41.3</v>
       </c>
-      <c r="D10">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
-        <v>1.387768817204301</v>
-      </c>
-      <c r="E10">
+        <v>1.0361264425489212</v>
+      </c>
+      <c r="F10" s="8">
+        <v>39.409999999999997</v>
+      </c>
+      <c r="G10" s="8">
         <v>42.29</v>
       </c>
-      <c r="F10">
+      <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>1.421034946236559</v>
-      </c>
-      <c r="G10">
+        <v>1.0730778990104035</v>
+      </c>
+      <c r="I10" s="8">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="J10" s="8">
         <v>41.86</v>
       </c>
-      <c r="H10">
+      <c r="K10" s="8">
         <f t="shared" si="2"/>
-        <v>1.4065860215053763</v>
-      </c>
-      <c r="I10">
+        <v>1.157632743362832</v>
+      </c>
+      <c r="L10" s="8">
+        <v>37.08</v>
+      </c>
+      <c r="M10" s="8">
         <v>41.32</v>
       </c>
-      <c r="J10">
+      <c r="N10" s="8">
         <f t="shared" si="3"/>
-        <v>1.3884408602150538</v>
-      </c>
-      <c r="K10">
+        <v>1.1143473570658038</v>
+      </c>
+      <c r="O10" s="8">
+        <v>38.65</v>
+      </c>
+      <c r="P10" s="8">
         <v>42.28</v>
       </c>
-      <c r="L10">
+      <c r="Q10" s="8">
         <f t="shared" si="4"/>
-        <v>1.4206989247311828</v>
-      </c>
-      <c r="M10">
+        <v>1.0939197930142304</v>
+      </c>
+      <c r="R10" s="8">
+        <v>38.29</v>
+      </c>
+      <c r="S10" s="8">
         <v>43.14</v>
       </c>
-      <c r="N10">
+      <c r="T10" s="8">
         <f t="shared" si="5"/>
-        <v>1.4495967741935483</v>
-      </c>
-      <c r="O10">
+        <v>1.1266649255680334</v>
+      </c>
+      <c r="U10" s="8">
+        <v>38.47</v>
+      </c>
+      <c r="V10" s="8">
         <v>44.1</v>
       </c>
-      <c r="P10">
+      <c r="W10">
         <f t="shared" si="6"/>
-        <v>1.4818548387096775</v>
-      </c>
-      <c r="Q10">
+        <v>1.1463478034832337</v>
+      </c>
+      <c r="X10">
         <v>417768</v>
       </c>
-      <c r="R10">
+      <c r="Y10">
         <v>519064</v>
       </c>
-      <c r="S10">
+      <c r="Z10">
         <v>588084</v>
       </c>
-      <c r="T10">
+      <c r="AA10">
         <v>512192</v>
       </c>
-      <c r="U10">
+      <c r="AB10">
         <v>539560</v>
       </c>
-      <c r="V10">
+      <c r="AC10">
         <v>520824</v>
       </c>
-      <c r="W10">
+      <c r="AD10">
         <v>555848</v>
       </c>
-      <c r="X10">
+      <c r="AE10">
         <v>575424</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>99</v>
       </c>
       <c r="B11">
         <v>44</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
+        <v>54.73</v>
+      </c>
+      <c r="D11" s="8">
         <v>69.88</v>
       </c>
-      <c r="D11">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
-        <v>1.5881818181818181</v>
-      </c>
-      <c r="E11">
+        <v>1.2768134478348254</v>
+      </c>
+      <c r="F11" s="8">
+        <v>25.35</v>
+      </c>
+      <c r="G11" s="8">
         <v>74.150000000000006</v>
       </c>
-      <c r="F11">
+      <c r="H11" s="8">
         <f t="shared" si="1"/>
-        <v>1.6852272727272728</v>
-      </c>
-      <c r="G11">
+        <v>2.9250493096646943</v>
+      </c>
+      <c r="I11" s="8">
+        <v>56.3</v>
+      </c>
+      <c r="J11" s="8">
         <v>72.14</v>
       </c>
-      <c r="H11">
+      <c r="K11" s="8">
         <f t="shared" si="2"/>
-        <v>1.6395454545454546</v>
-      </c>
-      <c r="I11">
+        <v>1.2813499111900533</v>
+      </c>
+      <c r="L11" s="8">
+        <v>52.08</v>
+      </c>
+      <c r="M11" s="8">
         <v>70.59</v>
       </c>
-      <c r="J11">
+      <c r="N11" s="8">
         <f t="shared" si="3"/>
-        <v>1.604318181818182</v>
-      </c>
-      <c r="K11">
+        <v>1.3554147465437789</v>
+      </c>
+      <c r="O11" s="8">
+        <v>53.79</v>
+      </c>
+      <c r="P11" s="8">
         <v>70.2</v>
       </c>
-      <c r="L11">
+      <c r="Q11" s="8">
         <f t="shared" si="4"/>
-        <v>1.5954545454545455</v>
-      </c>
-      <c r="M11">
+        <v>1.3050752928053542</v>
+      </c>
+      <c r="R11" s="8">
+        <v>54.77</v>
+      </c>
+      <c r="S11" s="8">
         <v>73.61</v>
       </c>
-      <c r="N11">
+      <c r="T11" s="8">
         <f t="shared" si="5"/>
-        <v>1.6729545454545454</v>
-      </c>
-      <c r="O11">
+        <v>1.3439839328099323</v>
+      </c>
+      <c r="U11" s="8">
+        <v>185.08</v>
+      </c>
+      <c r="V11" s="8">
         <v>628.19000000000005</v>
       </c>
-      <c r="P11">
+      <c r="W11">
         <f t="shared" si="6"/>
-        <v>14.277045454545457</v>
-      </c>
-      <c r="Q11">
+        <v>3.3941538794035013</v>
+      </c>
+      <c r="X11">
         <v>2525896</v>
       </c>
-      <c r="R11">
+      <c r="Y11">
         <v>2965116</v>
       </c>
-      <c r="S11">
+      <c r="Z11">
         <v>3103888</v>
       </c>
-      <c r="T11">
+      <c r="AA11">
         <v>2247020</v>
       </c>
-      <c r="U11">
+      <c r="AB11">
         <v>2181540</v>
       </c>
-      <c r="V11">
+      <c r="AC11">
         <v>2414916</v>
       </c>
-      <c r="W11">
+      <c r="AD11">
         <v>3600116</v>
       </c>
-      <c r="X11">
+      <c r="AE11">
         <v>2062376</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>100</v>
       </c>
       <c r="B12">
         <v>1.89</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
+        <v>1.61</v>
+      </c>
+      <c r="D12" s="8">
         <v>2.6</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
-        <v>1.3756613756613758</v>
-      </c>
-      <c r="E12">
+        <v>1.6149068322981366</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1.57</v>
+      </c>
+      <c r="G12" s="8">
         <v>2.33</v>
       </c>
-      <c r="F12">
+      <c r="H12" s="8">
         <f t="shared" si="1"/>
-        <v>1.232804232804233</v>
-      </c>
-      <c r="G12">
+        <v>1.484076433121019</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1.53</v>
+      </c>
+      <c r="J12" s="8">
         <v>2.4300000000000002</v>
       </c>
-      <c r="H12">
+      <c r="K12" s="8">
         <f t="shared" si="2"/>
-        <v>1.2857142857142858</v>
-      </c>
-      <c r="I12">
+        <v>1.5882352941176472</v>
+      </c>
+      <c r="L12" s="8">
+        <v>1.57</v>
+      </c>
+      <c r="M12" s="8">
         <v>2.39</v>
       </c>
-      <c r="J12">
+      <c r="N12" s="8">
         <f t="shared" si="3"/>
-        <v>1.2645502645502646</v>
-      </c>
-      <c r="K12">
+        <v>1.5222929936305734</v>
+      </c>
+      <c r="O12" s="8">
+        <v>1.58</v>
+      </c>
+      <c r="P12" s="8">
         <v>2.4500000000000002</v>
       </c>
-      <c r="L12">
+      <c r="Q12" s="8">
         <f t="shared" si="4"/>
-        <v>1.2962962962962965</v>
-      </c>
-      <c r="M12">
+        <v>1.5506329113924051</v>
+      </c>
+      <c r="R12" s="8">
+        <v>1.62</v>
+      </c>
+      <c r="S12" s="8">
         <v>2.58</v>
       </c>
-      <c r="N12">
+      <c r="T12" s="8">
         <f t="shared" si="5"/>
-        <v>1.3650793650793651</v>
-      </c>
-      <c r="O12">
+        <v>1.5925925925925926</v>
+      </c>
+      <c r="U12" s="8">
+        <v>1.65</v>
+      </c>
+      <c r="V12" s="8">
         <v>2.5</v>
       </c>
-      <c r="P12">
+      <c r="W12">
         <f t="shared" si="6"/>
-        <v>1.3227513227513228</v>
-      </c>
-      <c r="Q12">
+        <v>1.5151515151515151</v>
+      </c>
+      <c r="X12">
         <v>245192</v>
       </c>
-      <c r="R12">
+      <c r="Y12">
         <v>351252</v>
       </c>
-      <c r="S12">
+      <c r="Z12">
         <v>419504</v>
       </c>
-      <c r="T12">
+      <c r="AA12">
         <v>367764</v>
       </c>
-      <c r="U12">
+      <c r="AB12">
         <v>352768</v>
       </c>
-      <c r="V12">
+      <c r="AC12">
         <v>350168</v>
       </c>
-      <c r="W12">
+      <c r="AD12">
         <v>440200</v>
       </c>
-      <c r="X12">
+      <c r="AE12">
         <v>353760</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B13">
         <v>53.53</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
+        <v>54.54</v>
+      </c>
+      <c r="D13" s="8">
         <v>53.99</v>
       </c>
-      <c r="D13">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
-        <v>1.0085933121614048</v>
-      </c>
-      <c r="E13">
+        <v>0.98991565823248995</v>
+      </c>
+      <c r="F13" s="8">
+        <v>53.63</v>
+      </c>
+      <c r="G13" s="8">
         <v>55.22</v>
       </c>
-      <c r="F13">
+      <c r="H13" s="8">
         <f t="shared" si="1"/>
-        <v>1.0315710816364654</v>
-      </c>
-      <c r="G13">
+        <v>1.0296475853067313</v>
+      </c>
+      <c r="I13" s="8">
+        <v>54.33</v>
+      </c>
+      <c r="J13" s="8">
         <v>54.5</v>
       </c>
-      <c r="H13">
+      <c r="K13" s="8">
         <f t="shared" si="2"/>
-        <v>1.0181206799925275</v>
-      </c>
-      <c r="I13">
+        <v>1.0031290263206332</v>
+      </c>
+      <c r="L13" s="8">
+        <v>53.82</v>
+      </c>
+      <c r="M13" s="8">
         <v>55.01</v>
       </c>
-      <c r="J13">
+      <c r="N13" s="8">
         <f t="shared" si="3"/>
-        <v>1.0276480478236503</v>
-      </c>
-      <c r="K13">
+        <v>1.0221107395020439</v>
+      </c>
+      <c r="O13" s="8">
+        <v>54.73</v>
+      </c>
+      <c r="P13" s="8">
         <v>55.88</v>
       </c>
-      <c r="L13">
+      <c r="Q13" s="8">
         <f t="shared" si="4"/>
-        <v>1.0439006164767421</v>
-      </c>
-      <c r="M13">
+        <v>1.0210122419148548</v>
+      </c>
+      <c r="R13" s="8">
+        <v>54.71</v>
+      </c>
+      <c r="S13" s="8">
         <v>53.93</v>
       </c>
-      <c r="N13">
+      <c r="T13" s="8">
         <f t="shared" si="5"/>
-        <v>1.0074724453577433</v>
-      </c>
-      <c r="O13">
+        <v>0.98574300859075126</v>
+      </c>
+      <c r="U13" s="8">
+        <v>54.09</v>
+      </c>
+      <c r="V13" s="8">
         <v>54.18</v>
       </c>
-      <c r="P13">
+      <c r="W13">
         <f t="shared" si="6"/>
-        <v>1.012142723706333</v>
-      </c>
-      <c r="Q13">
+        <v>1.0016638935108153</v>
+      </c>
+      <c r="X13">
         <v>844712</v>
       </c>
-      <c r="R13">
+      <c r="Y13">
         <v>864292</v>
       </c>
-      <c r="S13">
+      <c r="Z13">
         <v>891144</v>
       </c>
-      <c r="T13">
+      <c r="AA13">
         <v>863160</v>
       </c>
-      <c r="U13">
+      <c r="AB13">
         <v>860192</v>
       </c>
-      <c r="V13">
+      <c r="AC13">
         <v>862940</v>
       </c>
-      <c r="W13">
+      <c r="AD13">
         <v>869724</v>
       </c>
-      <c r="X13">
+      <c r="AE13">
         <v>857508</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B14">
         <v>89.78</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
+        <v>93.62</v>
+      </c>
+      <c r="D14" s="8">
         <v>775.68</v>
       </c>
-      <c r="D14">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
-        <v>8.6397861439073278</v>
-      </c>
-      <c r="E14">
+        <v>8.2854091006195247</v>
+      </c>
+      <c r="F14" s="8">
+        <v>82.53</v>
+      </c>
+      <c r="G14" s="8">
         <v>777.46</v>
       </c>
-      <c r="F14">
+      <c r="H14" s="8">
         <f t="shared" si="1"/>
-        <v>8.659612385832034</v>
-      </c>
-      <c r="G14">
+        <v>9.420332000484672</v>
+      </c>
+      <c r="I14" s="8">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="J14" s="8">
         <v>847.68</v>
       </c>
-      <c r="H14">
+      <c r="K14" s="8">
         <f t="shared" si="2"/>
-        <v>9.4417464914234781</v>
-      </c>
-      <c r="I14">
+        <v>12.127038626609441</v>
+      </c>
+      <c r="L14" s="8">
+        <v>80.52</v>
+      </c>
+      <c r="M14" s="8">
         <v>891.82</v>
       </c>
-      <c r="J14">
+      <c r="N14" s="8">
         <f t="shared" si="3"/>
-        <v>9.9333927378035209</v>
-      </c>
-      <c r="K14">
+        <v>11.075757575757576</v>
+      </c>
+      <c r="O14" s="8">
+        <v>93.89</v>
+      </c>
+      <c r="P14" s="8">
         <v>775.13</v>
       </c>
-      <c r="L14">
+      <c r="Q14" s="8">
         <f t="shared" si="4"/>
-        <v>8.633660057919359</v>
-      </c>
-      <c r="M14">
+        <v>8.2557247843220782</v>
+      </c>
+      <c r="R14" s="8">
+        <v>86.02</v>
+      </c>
+      <c r="S14" s="8">
         <v>778.76</v>
       </c>
-      <c r="N14">
+      <c r="T14" s="8">
         <f t="shared" si="5"/>
-        <v>8.6740922254399635</v>
-      </c>
-      <c r="O14">
+        <v>9.0532434317600554</v>
+      </c>
+      <c r="U14" s="8">
+        <v>102.55</v>
+      </c>
+      <c r="V14" s="8">
         <v>1052.46</v>
       </c>
-      <c r="P14">
+      <c r="W14">
         <f t="shared" si="6"/>
-        <v>11.722655379817331</v>
-      </c>
-      <c r="Q14">
+        <v>10.262896148220381</v>
+      </c>
+      <c r="X14">
         <v>1161184</v>
       </c>
-      <c r="R14">
+      <c r="Y14">
         <v>1412792</v>
       </c>
-      <c r="S14">
+      <c r="Z14">
         <v>1912952</v>
       </c>
-      <c r="T14">
+      <c r="AA14">
         <v>1365684</v>
       </c>
-      <c r="U14">
+      <c r="AB14">
         <v>1396044</v>
       </c>
-      <c r="V14">
+      <c r="AC14">
         <v>1413956</v>
       </c>
-      <c r="W14">
+      <c r="AD14">
         <v>2013840</v>
       </c>
-      <c r="X14">
+      <c r="AE14">
         <v>2054448</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B15">
         <v>67.41</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
+        <v>53.67</v>
+      </c>
+      <c r="D15" s="8">
         <v>73.790000000000006</v>
       </c>
-      <c r="D15">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
-        <v>1.0946447114671416</v>
-      </c>
-      <c r="E15">
+        <v>1.3748835476057388</v>
+      </c>
+      <c r="F15" s="8">
+        <v>55.44</v>
+      </c>
+      <c r="G15" s="8">
         <v>74.36</v>
       </c>
-      <c r="F15">
+      <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>1.1031004302032339</v>
-      </c>
-      <c r="G15">
+        <v>1.3412698412698414</v>
+      </c>
+      <c r="I15" s="8">
+        <v>53.93</v>
+      </c>
+      <c r="J15" s="8">
         <v>71.319999999999993</v>
       </c>
-      <c r="H15">
+      <c r="K15" s="8">
         <f t="shared" si="2"/>
-        <v>1.0580032636107402</v>
-      </c>
-      <c r="I15">
+        <v>1.3224550343037269</v>
+      </c>
+      <c r="L15" s="8">
+        <v>54.17</v>
+      </c>
+      <c r="M15" s="8">
         <v>73.25</v>
       </c>
-      <c r="J15">
+      <c r="N15" s="8">
         <f t="shared" si="3"/>
-        <v>1.0866340305592643</v>
-      </c>
-      <c r="K15">
+        <v>1.352224478493631</v>
+      </c>
+      <c r="O15" s="8">
+        <v>53.57</v>
+      </c>
+      <c r="P15" s="8">
         <v>72.81</v>
       </c>
-      <c r="L15">
+      <c r="Q15" s="8">
         <f t="shared" si="4"/>
-        <v>1.0801068090787718</v>
-      </c>
-      <c r="M15">
+        <v>1.359156244166511</v>
+      </c>
+      <c r="R15" s="8">
+        <v>55.45</v>
+      </c>
+      <c r="S15" s="8">
         <v>74.95</v>
       </c>
-      <c r="N15">
+      <c r="T15" s="8">
         <f t="shared" si="5"/>
-        <v>1.1118528408248036</v>
-      </c>
-      <c r="O15">
+        <v>1.351668169522092</v>
+      </c>
+      <c r="U15" s="8">
+        <v>54.01</v>
+      </c>
+      <c r="V15" s="8">
         <v>72.8</v>
       </c>
-      <c r="P15">
+      <c r="W15">
         <f t="shared" si="6"/>
-        <v>1.0799584631360333</v>
-      </c>
-      <c r="Q15">
+        <v>1.347898537307906</v>
+      </c>
+      <c r="X15">
         <v>115852</v>
       </c>
-      <c r="R15">
+      <c r="Y15">
         <v>343464</v>
       </c>
-      <c r="S15">
+      <c r="Z15">
         <v>364988</v>
       </c>
-      <c r="T15">
+      <c r="AA15">
         <v>175424</v>
       </c>
-      <c r="U15">
+      <c r="AB15">
         <v>171856</v>
       </c>
-      <c r="V15">
+      <c r="AC15">
         <v>336376</v>
       </c>
-      <c r="W15">
+      <c r="AD15">
         <v>229104</v>
       </c>
-      <c r="X15">
+      <c r="AE15">
         <v>172664</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>104</v>
       </c>
       <c r="B16">
         <v>36.950000000000003</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="8">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="D16" s="8">
         <v>141.41</v>
       </c>
-      <c r="D16">
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
-        <v>3.8270635994587274</v>
-      </c>
-      <c r="E16">
+        <v>3.772945570971185</v>
+      </c>
+      <c r="F16" s="8">
+        <v>40.9</v>
+      </c>
+      <c r="G16" s="8">
         <v>190.13</v>
       </c>
-      <c r="F16">
+      <c r="H16" s="8">
         <f t="shared" si="1"/>
-        <v>5.145602165087956</v>
-      </c>
-      <c r="G16">
+        <v>4.6486552567237167</v>
+      </c>
+      <c r="I16" s="8">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="J16" s="8">
         <v>165.47</v>
       </c>
-      <c r="H16">
+      <c r="K16" s="8">
         <f t="shared" si="2"/>
-        <v>4.4782138024357234</v>
-      </c>
-      <c r="I16">
+        <v>4.3396275898242846</v>
+      </c>
+      <c r="L16" s="8">
+        <v>99.22</v>
+      </c>
+      <c r="M16" s="8">
         <v>397.46</v>
       </c>
-      <c r="J16">
+      <c r="N16" s="8">
         <f t="shared" si="3"/>
-        <v>10.756698240866033</v>
-      </c>
-      <c r="K16">
+        <v>4.005845595646039</v>
+      </c>
+      <c r="O16" s="8">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="P16" s="8">
         <v>238.99</v>
       </c>
-      <c r="L16">
+      <c r="Q16" s="8">
         <f t="shared" si="4"/>
-        <v>6.4679296346414068</v>
-      </c>
-      <c r="M16">
+        <v>6.3815754339118822</v>
+      </c>
+      <c r="R16" s="8">
+        <v>36.81</v>
+      </c>
+      <c r="S16" s="8">
         <v>174.12</v>
       </c>
-      <c r="N16">
+      <c r="T16" s="8">
         <f t="shared" si="5"/>
-        <v>4.7123139377537209</v>
-      </c>
-      <c r="O16">
+        <v>4.7302363488182557</v>
+      </c>
+      <c r="U16" s="8">
+        <v>163.43</v>
+      </c>
+      <c r="V16" s="8">
         <v>1230.3399999999999</v>
       </c>
-      <c r="P16">
+      <c r="W16">
         <f t="shared" si="6"/>
-        <v>33.29742895805142</v>
-      </c>
-      <c r="Q16">
+        <v>7.5282383895245664</v>
+      </c>
+      <c r="X16">
         <v>8608</v>
       </c>
-      <c r="R16">
+      <c r="Y16">
         <v>53464</v>
       </c>
-      <c r="S16">
+      <c r="Z16">
         <v>250668</v>
       </c>
-      <c r="T16">
+      <c r="AA16">
         <v>55040</v>
       </c>
-      <c r="U16">
+      <c r="AB16">
         <v>49396</v>
       </c>
-      <c r="V16">
+      <c r="AC16">
         <v>51512</v>
       </c>
-      <c r="W16">
+      <c r="AD16">
         <v>84284</v>
       </c>
-      <c r="X16">
+      <c r="AE16">
         <v>52040</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B17">
         <v>116.79</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="8">
+        <v>116.78</v>
+      </c>
+      <c r="D17" s="8">
         <v>313.12</v>
       </c>
-      <c r="D17">
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
-        <v>2.6810514598852642</v>
-      </c>
-      <c r="E17">
+        <v>2.681281041274191</v>
+      </c>
+      <c r="F17" s="8">
+        <v>115.89</v>
+      </c>
+      <c r="G17" s="8">
         <v>313.70999999999998</v>
       </c>
-      <c r="F17">
+      <c r="H17" s="8">
         <f t="shared" si="1"/>
-        <v>2.6861032622656045</v>
-      </c>
-      <c r="G17">
+        <v>2.7069634998705667</v>
+      </c>
+      <c r="I17" s="8">
+        <v>115.71</v>
+      </c>
+      <c r="J17" s="8">
         <v>295.43</v>
       </c>
-      <c r="H17">
+      <c r="K17" s="8">
         <f t="shared" si="2"/>
-        <v>2.5295830122441991</v>
-      </c>
-      <c r="I17">
+        <v>2.5531933281479562</v>
+      </c>
+      <c r="L17" s="8">
+        <v>119.32</v>
+      </c>
+      <c r="M17" s="8">
         <v>279.43</v>
       </c>
-      <c r="J17">
+      <c r="N17" s="8">
         <f t="shared" si="3"/>
-        <v>2.3925849815908897</v>
-      </c>
-      <c r="K17">
+        <v>2.3418538384177006</v>
+      </c>
+      <c r="O17" s="8">
+        <v>116.79</v>
+      </c>
+      <c r="P17" s="8">
         <v>312.57</v>
       </c>
-      <c r="L17">
+      <c r="Q17" s="8">
         <f t="shared" si="4"/>
         <v>2.6763421525815563</v>
       </c>
-      <c r="M17">
+      <c r="R17" s="8">
+        <v>116.35</v>
+      </c>
+      <c r="S17" s="8">
         <v>306.41000000000003</v>
       </c>
-      <c r="N17">
+      <c r="T17" s="8">
         <f t="shared" si="5"/>
-        <v>2.6235979107800325</v>
-      </c>
-      <c r="O17">
+        <v>2.6335195530726261</v>
+      </c>
+      <c r="U17" s="8">
+        <v>121.99</v>
+      </c>
+      <c r="V17" s="8">
         <v>322.93</v>
       </c>
-      <c r="P17">
+      <c r="W17">
         <f t="shared" si="6"/>
-        <v>2.7650483774295744</v>
-      </c>
-      <c r="Q17">
+        <v>2.6471841954258548</v>
+      </c>
+      <c r="X17">
         <v>31548</v>
       </c>
-      <c r="R17">
+      <c r="Y17">
         <v>50344</v>
       </c>
-      <c r="S17">
+      <c r="Z17">
         <v>79232</v>
       </c>
-      <c r="T17">
+      <c r="AA17">
         <v>52752</v>
       </c>
-      <c r="U17">
+      <c r="AB17">
         <v>62408</v>
       </c>
-      <c r="V17">
+      <c r="AC17">
         <v>49216</v>
       </c>
-      <c r="W17">
+      <c r="AD17">
         <v>48996</v>
       </c>
-      <c r="X17">
+      <c r="AE17">
         <v>76096</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>106</v>
       </c>
       <c r="B18">
         <v>52.74</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="8">
+        <v>50.64</v>
+      </c>
+      <c r="D18" s="8">
         <v>66.790000000000006</v>
       </c>
-      <c r="D18">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
-        <v>1.2664012135001896</v>
-      </c>
-      <c r="E18">
+        <v>1.31891785150079</v>
+      </c>
+      <c r="F18" s="8">
+        <v>50.77</v>
+      </c>
+      <c r="G18" s="8">
         <v>66.81</v>
       </c>
-      <c r="F18">
+      <c r="H18" s="8">
         <f t="shared" si="1"/>
-        <v>1.2667804323094425</v>
-      </c>
-      <c r="G18">
+        <v>1.3159346070514082</v>
+      </c>
+      <c r="I18" s="8">
+        <v>50.46</v>
+      </c>
+      <c r="J18" s="8">
         <v>66.819999999999993</v>
       </c>
-      <c r="H18">
+      <c r="K18" s="8">
         <f t="shared" si="2"/>
-        <v>1.2669700417140688</v>
-      </c>
-      <c r="I18">
+        <v>1.3242172017439555</v>
+      </c>
+      <c r="L18" s="8">
+        <v>50.45</v>
+      </c>
+      <c r="M18" s="8">
         <v>66.17</v>
       </c>
-      <c r="J18">
+      <c r="N18" s="8">
         <f t="shared" si="3"/>
-        <v>1.2546454304133485</v>
-      </c>
-      <c r="K18">
+        <v>1.3115956392467789</v>
+      </c>
+      <c r="O18" s="8">
+        <v>50.66</v>
+      </c>
+      <c r="P18" s="8">
         <v>66.540000000000006</v>
       </c>
-      <c r="L18">
+      <c r="Q18" s="8">
         <f t="shared" si="4"/>
-        <v>1.2616609783845278</v>
-      </c>
-      <c r="M18">
+        <v>1.3134622976707464</v>
+      </c>
+      <c r="R18" s="8">
+        <v>50.28</v>
+      </c>
+      <c r="S18" s="8">
         <v>65.91</v>
       </c>
-      <c r="N18">
+      <c r="T18" s="8">
         <f t="shared" si="5"/>
-        <v>1.2497155858930602</v>
-      </c>
-      <c r="O18">
+        <v>1.3108591885441527</v>
+      </c>
+      <c r="U18" s="8">
+        <v>50.92</v>
+      </c>
+      <c r="V18" s="8">
         <v>66.64</v>
       </c>
-      <c r="P18">
+      <c r="W18">
         <f t="shared" si="6"/>
-        <v>1.2635570724307925</v>
-      </c>
-      <c r="Q18">
+        <v>1.3087195600942654</v>
+      </c>
+      <c r="X18">
         <v>496328</v>
       </c>
-      <c r="R18">
+      <c r="Y18">
         <v>854632</v>
       </c>
-      <c r="S18">
+      <c r="Z18">
         <v>1662308</v>
       </c>
-      <c r="T18">
+      <c r="AA18">
         <v>969468</v>
       </c>
-      <c r="U18">
+      <c r="AB18">
         <v>915092</v>
       </c>
-      <c r="V18">
+      <c r="AC18">
         <v>843284</v>
       </c>
-      <c r="W18">
+      <c r="AD18">
         <v>1048964</v>
       </c>
-      <c r="X18">
+      <c r="AE18">
         <v>950592</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B19">
         <f>AVERAGE(B4:B18)</f>
         <v>49.301333333333332</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:O19" si="7">AVERAGE(C4:C18)</f>
+        <f t="shared" ref="C19:V19" si="7">AVERAGE(C4:C18)</f>
+        <v>50.902666666666661</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="7"/>
         <v>159.61000000000001</v>
       </c>
-      <c r="D19">
-        <f>AVERAGE(D4:D18)</f>
-        <v>2.9166132044655511</v>
-      </c>
-      <c r="E19">
+      <c r="E19" s="16">
+        <f>AVERAGE(E4:E18)</f>
+        <v>2.8008415003256957</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>47.982666666666667</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="7"/>
         <v>162.92799999999997</v>
       </c>
-      <c r="F19">
-        <f>AVERAGE(F4:F18)</f>
-        <v>3.0054373615495269</v>
-      </c>
-      <c r="G19">
+      <c r="H19" s="16">
+        <f>G19/F19</f>
+        <v>3.3955595075999661</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>48.876666666666665</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="7"/>
         <v>166.02199999999999</v>
       </c>
-      <c r="H19">
-        <f>AVERAGE(H4:H18)</f>
-        <v>3.0108951759660334</v>
-      </c>
-      <c r="I19">
+      <c r="K19" s="16">
+        <f>AVERAGE(K4:K18)</f>
+        <v>3.1988199407017373</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="7"/>
+        <v>55.282000000000004</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="7"/>
         <v>219.45933333333332</v>
       </c>
-      <c r="J19">
-        <f>AVERAGE(J4:J18)</f>
-        <v>5.9958208521882792</v>
-      </c>
-      <c r="K19">
+      <c r="N19" s="16">
+        <f>AVERAGE(N4:N18)</f>
+        <v>4.1855415815764339</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>50.98</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="7"/>
         <v>166.73533333333336</v>
       </c>
-      <c r="L19">
-        <f>AVERAGE(L4:L18)</f>
-        <v>3.1473722591707083</v>
-      </c>
-      <c r="M19">
+      <c r="Q19" s="16">
+        <f>AVERAGE(Q4:Q18)</f>
+        <v>2.9366767749739626</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="7"/>
+        <v>50.011333333333333</v>
+      </c>
+      <c r="S19">
         <f t="shared" si="7"/>
         <v>162.51733333333331</v>
       </c>
-      <c r="N19">
-        <f>AVERAGE(N4:N18)</f>
-        <v>2.9957046900597746</v>
-      </c>
-      <c r="O19">
+      <c r="T19" s="16">
+        <f>AVERAGE(T4:T18)</f>
+        <v>3.023912018606818</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="7"/>
+        <v>72.940000000000012</v>
+      </c>
+      <c r="V19">
         <f t="shared" si="7"/>
         <v>333.83866666666671</v>
       </c>
-      <c r="P19">
-        <f>AVERAGE(P4:P18)</f>
-        <v>7.4616960338396439</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>110</v>
+      <c r="W19" s="16">
+        <f>AVERAGE(W4:W18)</f>
+        <v>3.7238252768344609</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="Q2:X2"/>
-    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="B2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5998,7 +6385,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>